<commit_message>
Added MeetID column and Added DateTime Field
</commit_message>
<xml_diff>
--- a/Excel File Manual Tests/SearchResultsTable.xlsx
+++ b/Excel File Manual Tests/SearchResultsTable.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23117"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="1380" yWindow="2300" windowWidth="25600" windowHeight="14980"/>
   </bookViews>
   <sheets>
-    <sheet name="SearchResultsTable" sheetId="1" r:id="rId4"/>
+    <sheet name="SearchResultsTable" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="599">
   <si>
     <t>id</t>
   </si>
@@ -1845,54 +1849,81 @@
   </si>
   <si>
     <t>http://app05.ottawa.ca/sirepub/view.aspx?cabinet=published_meetings&amp;doctype=SUMMARY&amp;folderid=4880</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>MeetID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
-      <strike val="0"/>
-      <color rgb="FF000000"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -2180,19 +2211,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:M87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2206,34 +2234,40 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>597</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="O1" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2246,33 +2280,39 @@
       <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="str">
+        <f>C2&amp;" - "&amp;D2</f>
+        <v>2012-Jun-18 - 9:30 AM</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
       <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="M2"/>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="O2">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2285,33 +2325,39 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E66" si="0">C3&amp;" - "&amp;D3</f>
+        <v>2012-Jun-19 - 9:30 AM</v>
+      </c>
+      <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
       <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>29</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>30</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>31</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>32</v>
       </c>
-      <c r="M3"/>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="O3">
+        <v>2407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2324,33 +2370,39 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Jun-20 - 9:30 AM</v>
+      </c>
+      <c r="F4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
       <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
         <v>36</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>37</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>38</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>39</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>40</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>41</v>
       </c>
-      <c r="M4"/>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="O4">
+        <v>2147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2363,33 +2415,39 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Jun-21 - 9:30 AM</v>
+      </c>
+      <c r="F5" t="s">
         <v>44</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
       <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
         <v>45</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>46</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>47</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>48</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>49</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>50</v>
       </c>
-      <c r="M5"/>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="O5">
+        <v>2154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2402,29 +2460,33 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Jun-21 - 9:30 AM</v>
+      </c>
+      <c r="F6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
       <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
         <v>52</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>53</v>
       </c>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>54</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>55</v>
       </c>
-      <c r="M6"/>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="O6">
+        <v>2409</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2437,33 +2499,39 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Jun-25 - 9:30 AM</v>
+      </c>
+      <c r="F7" t="s">
         <v>58</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
       <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
         <v>59</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>60</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>61</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>62</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>63</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>64</v>
       </c>
-      <c r="M7"/>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="O7">
+        <v>2211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2476,33 +2544,39 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Jun-26 - 9:30 AM</v>
+      </c>
+      <c r="F8" t="s">
         <v>67</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
       <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
         <v>68</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>69</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>70</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>71</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>72</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>73</v>
       </c>
-      <c r="M8"/>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="O8">
+        <v>2181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2515,29 +2589,33 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Jun-27 - 9:30 AM</v>
+      </c>
+      <c r="F9" t="s">
         <v>76</v>
       </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
       <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
         <v>77</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>78</v>
       </c>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>79</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>80</v>
       </c>
-      <c r="M9"/>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="O9">
+        <v>2484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2550,33 +2628,39 @@
       <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Jul-03 - 9:30 AM</v>
+      </c>
+      <c r="F10" t="s">
         <v>83</v>
       </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
       <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
         <v>84</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>85</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>86</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>87</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>88</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>89</v>
       </c>
-      <c r="M10"/>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="O10">
+        <v>2412</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2589,33 +2673,39 @@
       <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Jul-04 - 9:30 AM</v>
+      </c>
+      <c r="F11" t="s">
         <v>92</v>
       </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
       <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
         <v>93</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>94</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>95</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>96</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>97</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>98</v>
       </c>
-      <c r="M11"/>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="O11">
+        <v>2411</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2628,33 +2718,39 @@
       <c r="D12" t="s">
         <v>15</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Jul-06 - 9:30 AM</v>
+      </c>
+      <c r="F12" t="s">
         <v>100</v>
       </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
       <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
         <v>101</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>102</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>103</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>104</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>105</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>106</v>
       </c>
-      <c r="M12"/>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="O12">
+        <v>2216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2667,33 +2763,39 @@
       <c r="D13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Jul-09 - 9:30 AM</v>
+      </c>
+      <c r="F13" t="s">
         <v>108</v>
       </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
       <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
         <v>109</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>110</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>111</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>112</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>113</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>114</v>
       </c>
-      <c r="M13"/>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="O13">
+        <v>2362</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2706,29 +2808,33 @@
       <c r="D14" t="s">
         <v>116</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Jul-11 - 10:00 AM</v>
+      </c>
+      <c r="F14" t="s">
         <v>117</v>
       </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
       <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
         <v>118</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>119</v>
       </c>
-      <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>120</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>121</v>
       </c>
-      <c r="M14"/>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="O14">
+        <v>2487</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2741,29 +2847,33 @@
       <c r="D15" t="s">
         <v>123</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Aug-02 - 6:00 PM</v>
+      </c>
+      <c r="F15" t="s">
         <v>124</v>
       </c>
-      <c r="F15" t="s">
-        <v>17</v>
-      </c>
       <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="s">
         <v>125</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>126</v>
       </c>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>127</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>128</v>
       </c>
-      <c r="M15"/>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="O15">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2776,33 +2886,39 @@
       <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Aug-23 - 9:30 AM</v>
+      </c>
+      <c r="F16" t="s">
         <v>130</v>
       </c>
-      <c r="F16" t="s">
-        <v>17</v>
-      </c>
       <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" t="s">
         <v>131</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>132</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>133</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>134</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>135</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>136</v>
       </c>
-      <c r="M16"/>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="O16">
+        <v>2361</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2815,33 +2931,39 @@
       <c r="D17" t="s">
         <v>15</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Aug-24 - 9:30 AM</v>
+      </c>
+      <c r="F17" t="s">
         <v>138</v>
       </c>
-      <c r="F17" t="s">
-        <v>17</v>
-      </c>
       <c r="G17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" t="s">
         <v>139</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>140</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>141</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>142</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>143</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>144</v>
       </c>
-      <c r="M17"/>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="O17">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2854,33 +2976,39 @@
       <c r="D18" t="s">
         <v>15</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Aug-27 - 9:30 AM</v>
+      </c>
+      <c r="F18" t="s">
         <v>100</v>
       </c>
-      <c r="F18" t="s">
-        <v>17</v>
-      </c>
       <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" t="s">
         <v>146</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>147</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>148</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>149</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>150</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>151</v>
       </c>
-      <c r="M18"/>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="O18">
+        <v>2143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2893,33 +3021,39 @@
       <c r="D19" t="s">
         <v>15</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Aug-28 - 9:30 AM</v>
+      </c>
+      <c r="F19" t="s">
         <v>153</v>
       </c>
-      <c r="F19" t="s">
-        <v>17</v>
-      </c>
       <c r="G19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" t="s">
         <v>154</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>155</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>156</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>157</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>158</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>159</v>
       </c>
-      <c r="M19"/>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="O19">
+        <v>2213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2932,25 +3066,27 @@
       <c r="D20" t="s">
         <v>116</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Aug-28 - 10:00 AM</v>
+      </c>
+      <c r="F20" t="s">
         <v>161</v>
       </c>
-      <c r="F20" t="s">
-        <v>17</v>
-      </c>
       <c r="G20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" t="s">
         <v>162</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>163</v>
       </c>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="O20">
+        <v>2221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2963,29 +3099,33 @@
       <c r="D21" t="s">
         <v>116</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Aug-29 - 10:00 AM</v>
+      </c>
+      <c r="F21" t="s">
         <v>165</v>
       </c>
-      <c r="F21" t="s">
-        <v>17</v>
-      </c>
       <c r="G21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" t="s">
         <v>166</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>167</v>
       </c>
-      <c r="I21"/>
-      <c r="J21"/>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>168</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>169</v>
       </c>
-      <c r="M21"/>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="O21">
+        <v>2151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2998,33 +3138,39 @@
       <c r="D22" t="s">
         <v>15</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Aug-30 - 9:30 AM</v>
+      </c>
+      <c r="F22" t="s">
         <v>171</v>
       </c>
-      <c r="F22" t="s">
-        <v>17</v>
-      </c>
       <c r="G22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" t="s">
         <v>172</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>173</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>174</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>175</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>176</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>177</v>
       </c>
-      <c r="M22"/>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="O22">
+        <v>2219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3037,33 +3183,39 @@
       <c r="D23" t="s">
         <v>15</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Sep-05 - 9:30 AM</v>
+      </c>
+      <c r="F23" t="s">
         <v>16</v>
       </c>
-      <c r="F23" t="s">
-        <v>17</v>
-      </c>
       <c r="G23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" t="s">
         <v>179</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>180</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>181</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>182</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>183</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>184</v>
       </c>
-      <c r="M23"/>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="O23">
+        <v>2121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3076,33 +3228,39 @@
       <c r="D24" t="s">
         <v>15</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Sep-06 - 9:30 AM</v>
+      </c>
+      <c r="F24" t="s">
         <v>44</v>
       </c>
-      <c r="F24" t="s">
-        <v>17</v>
-      </c>
       <c r="G24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" t="s">
         <v>186</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>187</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>188</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>189</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>190</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>191</v>
       </c>
-      <c r="M24"/>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="O24">
+        <v>2364</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3115,33 +3273,39 @@
       <c r="D25" t="s">
         <v>15</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Sep-11 - 9:30 AM</v>
+      </c>
+      <c r="F25" t="s">
         <v>108</v>
       </c>
-      <c r="F25" t="s">
-        <v>17</v>
-      </c>
       <c r="G25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" t="s">
         <v>193</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>194</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>195</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>196</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>197</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>198</v>
       </c>
-      <c r="M25"/>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="O25">
+        <v>2360</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3154,33 +3318,39 @@
       <c r="D26" t="s">
         <v>15</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Sep-12 - 9:30 AM</v>
+      </c>
+      <c r="F26" t="s">
         <v>200</v>
       </c>
-      <c r="F26" t="s">
-        <v>17</v>
-      </c>
       <c r="G26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" t="s">
         <v>201</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>202</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>203</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>204</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>205</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>206</v>
       </c>
-      <c r="M26"/>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="O26">
+        <v>2408</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3193,33 +3363,39 @@
       <c r="D27" t="s">
         <v>15</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Sep-13 - 9:30 AM</v>
+      </c>
+      <c r="F27" t="s">
         <v>100</v>
       </c>
-      <c r="F27" t="s">
-        <v>17</v>
-      </c>
       <c r="G27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" t="s">
         <v>209</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>210</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>211</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>212</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>213</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>214</v>
       </c>
-      <c r="M27"/>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="O27">
+        <v>2204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3232,33 +3408,39 @@
       <c r="D28" t="s">
         <v>15</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Sep-17 - 9:30 AM</v>
+      </c>
+      <c r="F28" t="s">
         <v>216</v>
       </c>
-      <c r="F28" t="s">
-        <v>17</v>
-      </c>
       <c r="G28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" t="s">
         <v>217</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>218</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>219</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>220</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>221</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>222</v>
       </c>
-      <c r="M28"/>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="O28">
+        <v>2275</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3271,33 +3453,39 @@
       <c r="D29" t="s">
         <v>15</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Sep-19 - 9:30 AM</v>
+      </c>
+      <c r="F29" t="s">
         <v>100</v>
       </c>
-      <c r="F29" t="s">
-        <v>17</v>
-      </c>
       <c r="G29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" t="s">
         <v>224</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>225</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>226</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>227</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>228</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>229</v>
       </c>
-      <c r="M29"/>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="O29">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3310,33 +3498,39 @@
       <c r="D30" t="s">
         <v>15</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Sep-20 - 9:30 AM</v>
+      </c>
+      <c r="F30" t="s">
         <v>44</v>
       </c>
-      <c r="F30" t="s">
-        <v>17</v>
-      </c>
       <c r="G30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" t="s">
         <v>231</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>232</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>233</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>234</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>235</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>236</v>
       </c>
-      <c r="M30"/>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="O30">
+        <v>2363</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3349,29 +3543,33 @@
       <c r="D31" t="s">
         <v>123</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Sep-20 - 6:00 PM</v>
+      </c>
+      <c r="F31" t="s">
         <v>124</v>
       </c>
-      <c r="F31" t="s">
-        <v>17</v>
-      </c>
       <c r="G31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" t="s">
         <v>237</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>238</v>
       </c>
-      <c r="I31"/>
-      <c r="J31"/>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>239</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>240</v>
       </c>
-      <c r="M31"/>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="O31">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3384,33 +3582,39 @@
       <c r="D32" t="s">
         <v>15</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Sep-25 - 9:30 AM</v>
+      </c>
+      <c r="F32" t="s">
         <v>108</v>
       </c>
-      <c r="F32" t="s">
-        <v>17</v>
-      </c>
       <c r="G32" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" t="s">
         <v>242</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>243</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>244</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>245</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>246</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>247</v>
       </c>
-      <c r="M32"/>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="O32">
+        <v>2349</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3423,33 +3627,39 @@
       <c r="D33" t="s">
         <v>15</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Sep-26 - 9:30 AM</v>
+      </c>
+      <c r="F33" t="s">
         <v>249</v>
       </c>
-      <c r="F33" t="s">
-        <v>17</v>
-      </c>
       <c r="G33" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" t="s">
         <v>250</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>251</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>252</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>253</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>254</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>255</v>
       </c>
-      <c r="M33"/>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="O33">
+        <v>2404</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3462,33 +3672,39 @@
       <c r="D34" t="s">
         <v>15</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Sep-27 - 9:30 AM</v>
+      </c>
+      <c r="F34" t="s">
         <v>257</v>
       </c>
-      <c r="F34" t="s">
-        <v>17</v>
-      </c>
       <c r="G34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" t="s">
         <v>258</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>259</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>260</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>261</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>262</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>263</v>
       </c>
-      <c r="M34"/>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="O34">
+        <v>2218</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3501,33 +3717,39 @@
       <c r="D35" t="s">
         <v>15</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Oct-02 - 9:30 AM</v>
+      </c>
+      <c r="F35" t="s">
         <v>265</v>
       </c>
-      <c r="F35" t="s">
-        <v>17</v>
-      </c>
       <c r="G35" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" t="s">
         <v>266</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>267</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>268</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>269</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>270</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>271</v>
       </c>
-      <c r="M35"/>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="O35">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3540,33 +3762,39 @@
       <c r="D36" t="s">
         <v>15</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Oct-03 - 9:30 AM</v>
+      </c>
+      <c r="F36" t="s">
         <v>92</v>
       </c>
-      <c r="F36" t="s">
-        <v>17</v>
-      </c>
       <c r="G36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" t="s">
         <v>273</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>274</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>275</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>276</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>277</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>278</v>
       </c>
-      <c r="M36"/>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="O36">
+        <v>2285</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3579,33 +3807,39 @@
       <c r="D37" t="s">
         <v>280</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Oct-04 - 7:00 PM</v>
+      </c>
+      <c r="F37" t="s">
         <v>44</v>
       </c>
-      <c r="F37" t="s">
-        <v>17</v>
-      </c>
       <c r="G37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" t="s">
         <v>281</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>282</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>283</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>284</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>285</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
         <v>286</v>
       </c>
-      <c r="M37"/>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="O37">
+        <v>2206</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3618,33 +3852,39 @@
       <c r="D38" t="s">
         <v>15</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Oct-09 - 9:30 AM</v>
+      </c>
+      <c r="F38" t="s">
         <v>108</v>
       </c>
-      <c r="F38" t="s">
-        <v>17</v>
-      </c>
       <c r="G38" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" t="s">
         <v>288</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>289</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>290</v>
       </c>
-      <c r="J38" t="s">
+      <c r="K38" t="s">
         <v>291</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>292</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>293</v>
       </c>
-      <c r="M38"/>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="O38">
+        <v>2284</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3657,29 +3897,33 @@
       <c r="D39" t="s">
         <v>116</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Oct-10 - 10:00 AM</v>
+      </c>
+      <c r="F39" t="s">
         <v>249</v>
       </c>
-      <c r="F39" t="s">
-        <v>17</v>
-      </c>
       <c r="G39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" t="s">
         <v>295</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>296</v>
       </c>
-      <c r="I39"/>
-      <c r="J39"/>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>297</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>298</v>
       </c>
-      <c r="M39"/>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="O39">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3692,33 +3936,39 @@
       <c r="D40" t="s">
         <v>15</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Oct-15 - 9:30 AM</v>
+      </c>
+      <c r="F40" t="s">
         <v>16</v>
       </c>
-      <c r="F40" t="s">
-        <v>17</v>
-      </c>
       <c r="G40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H40" t="s">
         <v>300</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>301</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>302</v>
       </c>
-      <c r="J40" t="s">
+      <c r="K40" t="s">
         <v>303</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
         <v>304</v>
       </c>
-      <c r="L40" t="s">
+      <c r="M40" t="s">
         <v>305</v>
       </c>
-      <c r="M40"/>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="O40">
+        <v>2149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3731,33 +3981,39 @@
       <c r="D41" t="s">
         <v>15</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Oct-16 - 9:30 AM</v>
+      </c>
+      <c r="F41" t="s">
         <v>26</v>
       </c>
-      <c r="F41" t="s">
-        <v>17</v>
-      </c>
       <c r="G41" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" t="s">
         <v>307</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>308</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>309</v>
       </c>
-      <c r="J41" t="s">
+      <c r="K41" t="s">
         <v>310</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>311</v>
       </c>
-      <c r="L41" t="s">
+      <c r="M41" t="s">
         <v>312</v>
       </c>
-      <c r="M41"/>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="O41">
+        <v>2229</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3770,33 +4026,39 @@
       <c r="D42" t="s">
         <v>15</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Oct-17 - 9:30 AM</v>
+      </c>
+      <c r="F42" t="s">
         <v>26</v>
       </c>
-      <c r="F42" t="s">
-        <v>17</v>
-      </c>
       <c r="G42" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" t="s">
         <v>314</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>315</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>316</v>
       </c>
-      <c r="J42" t="s">
+      <c r="K42" t="s">
         <v>317</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>318</v>
       </c>
-      <c r="L42" t="s">
+      <c r="M42" t="s">
         <v>319</v>
       </c>
-      <c r="M42"/>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="O42">
+        <v>2230</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3809,33 +4071,39 @@
       <c r="D43" t="s">
         <v>15</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Oct-18 - 9:30 AM</v>
+      </c>
+      <c r="F43" t="s">
         <v>26</v>
       </c>
-      <c r="F43" t="s">
-        <v>17</v>
-      </c>
       <c r="G43" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" t="s">
         <v>321</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>322</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
         <v>323</v>
       </c>
-      <c r="J43" t="s">
+      <c r="K43" t="s">
         <v>324</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>325</v>
       </c>
-      <c r="L43" t="s">
+      <c r="M43" t="s">
         <v>326</v>
       </c>
-      <c r="M43"/>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="O43">
+        <v>2237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3848,29 +4116,33 @@
       <c r="D44" t="s">
         <v>123</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Oct-18 - 6:00 PM</v>
+      </c>
+      <c r="F44" t="s">
         <v>124</v>
       </c>
-      <c r="F44" t="s">
-        <v>17</v>
-      </c>
       <c r="G44" t="s">
+        <v>17</v>
+      </c>
+      <c r="H44" t="s">
         <v>327</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>328</v>
       </c>
-      <c r="I44"/>
-      <c r="J44"/>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
         <v>329</v>
       </c>
-      <c r="L44" t="s">
+      <c r="M44" t="s">
         <v>330</v>
       </c>
-      <c r="M44"/>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="O44">
+        <v>2176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3883,33 +4155,39 @@
       <c r="D45" t="s">
         <v>15</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Oct-23 - 9:30 AM</v>
+      </c>
+      <c r="F45" t="s">
         <v>26</v>
       </c>
-      <c r="F45" t="s">
-        <v>17</v>
-      </c>
       <c r="G45" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" t="s">
         <v>332</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>333</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
         <v>334</v>
       </c>
-      <c r="J45" t="s">
+      <c r="K45" t="s">
         <v>335</v>
       </c>
-      <c r="K45" t="s">
+      <c r="L45" t="s">
         <v>336</v>
       </c>
-      <c r="L45" t="s">
+      <c r="M45" t="s">
         <v>337</v>
       </c>
-      <c r="M45"/>
-    </row>
-    <row r="46" spans="1:13">
+      <c r="O45">
+        <v>2245</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3922,25 +4200,27 @@
       <c r="D46" t="s">
         <v>116</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Oct-24 - 10:00 AM</v>
+      </c>
+      <c r="F46" t="s">
         <v>117</v>
       </c>
-      <c r="F46" t="s">
-        <v>17</v>
-      </c>
       <c r="G46" t="s">
+        <v>17</v>
+      </c>
+      <c r="H46" t="s">
         <v>339</v>
       </c>
-      <c r="H46" t="s">
+      <c r="I46" t="s">
         <v>340</v>
       </c>
-      <c r="I46"/>
-      <c r="J46"/>
-      <c r="K46"/>
-      <c r="L46"/>
-      <c r="M46"/>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="O46">
+        <v>2495</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3953,33 +4233,39 @@
       <c r="D47" t="s">
         <v>341</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Oct-24 - 3:30 PM</v>
+      </c>
+      <c r="F47" t="s">
         <v>257</v>
       </c>
-      <c r="F47" t="s">
-        <v>17</v>
-      </c>
       <c r="G47" t="s">
+        <v>17</v>
+      </c>
+      <c r="H47" t="s">
         <v>342</v>
       </c>
-      <c r="H47" t="s">
+      <c r="I47" t="s">
         <v>343</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>344</v>
       </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
         <v>345</v>
       </c>
-      <c r="K47" t="s">
+      <c r="L47" t="s">
         <v>346</v>
       </c>
-      <c r="L47" t="s">
+      <c r="M47" t="s">
         <v>347</v>
       </c>
-      <c r="M47"/>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="O47">
+        <v>2236</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3992,33 +4278,39 @@
       <c r="D48" t="s">
         <v>15</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Nov-01 - 9:30 AM</v>
+      </c>
+      <c r="F48" t="s">
         <v>44</v>
       </c>
-      <c r="F48" t="s">
-        <v>17</v>
-      </c>
       <c r="G48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" t="s">
         <v>349</v>
       </c>
-      <c r="H48" t="s">
+      <c r="I48" t="s">
         <v>350</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>351</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
         <v>352</v>
       </c>
-      <c r="K48" t="s">
+      <c r="L48" t="s">
         <v>353</v>
       </c>
-      <c r="L48" t="s">
+      <c r="M48" t="s">
         <v>354</v>
       </c>
-      <c r="M48"/>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="O48">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4031,25 +4323,27 @@
       <c r="D49" t="s">
         <v>15</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Nov-01 - 9:30 AM</v>
+      </c>
+      <c r="F49" t="s">
         <v>124</v>
       </c>
-      <c r="F49" t="s">
-        <v>17</v>
-      </c>
       <c r="G49" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" t="s">
         <v>356</v>
       </c>
-      <c r="H49" t="s">
+      <c r="I49" t="s">
         <v>357</v>
       </c>
-      <c r="I49"/>
-      <c r="J49"/>
-      <c r="K49"/>
-      <c r="L49"/>
-      <c r="M49"/>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="O49">
+        <v>2397</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4062,33 +4356,39 @@
       <c r="D50" t="s">
         <v>15</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Nov-06 - 9:30 AM</v>
+      </c>
+      <c r="F50" t="s">
         <v>83</v>
       </c>
-      <c r="F50" t="s">
-        <v>17</v>
-      </c>
       <c r="G50" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" t="s">
         <v>359</v>
       </c>
-      <c r="H50" t="s">
+      <c r="I50" t="s">
         <v>360</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" t="s">
         <v>361</v>
       </c>
-      <c r="J50" t="s">
+      <c r="K50" t="s">
         <v>362</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>363</v>
       </c>
-      <c r="L50" t="s">
+      <c r="M50" t="s">
         <v>364</v>
       </c>
-      <c r="M50"/>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="O50">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4101,33 +4401,39 @@
       <c r="D51" t="s">
         <v>15</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Nov-07 - 9:30 AM</v>
+      </c>
+      <c r="F51" t="s">
         <v>16</v>
       </c>
-      <c r="F51" t="s">
-        <v>17</v>
-      </c>
       <c r="G51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H51" t="s">
         <v>366</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
         <v>367</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J51" t="s">
         <v>368</v>
       </c>
-      <c r="J51" t="s">
+      <c r="K51" t="s">
         <v>369</v>
       </c>
-      <c r="K51" t="s">
+      <c r="L51" t="s">
         <v>370</v>
       </c>
-      <c r="L51" t="s">
+      <c r="M51" t="s">
         <v>371</v>
       </c>
-      <c r="M51"/>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="O51">
+        <v>2178</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4140,33 +4446,39 @@
       <c r="D52" t="s">
         <v>15</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Nov-13 - 9:30 AM</v>
+      </c>
+      <c r="F52" t="s">
         <v>130</v>
       </c>
-      <c r="F52" t="s">
-        <v>17</v>
-      </c>
       <c r="G52" t="s">
+        <v>17</v>
+      </c>
+      <c r="H52" t="s">
         <v>373</v>
       </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
         <v>374</v>
       </c>
-      <c r="I52" t="s">
+      <c r="J52" t="s">
         <v>375</v>
       </c>
-      <c r="J52" t="s">
+      <c r="K52" t="s">
         <v>376</v>
       </c>
-      <c r="K52" t="s">
+      <c r="L52" t="s">
         <v>377</v>
       </c>
-      <c r="L52" t="s">
+      <c r="M52" t="s">
         <v>378</v>
       </c>
-      <c r="M52"/>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="O52">
+        <v>2266</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4179,29 +4491,33 @@
       <c r="D53" t="s">
         <v>116</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Nov-14 - 10:00 AM</v>
+      </c>
+      <c r="F53" t="s">
         <v>249</v>
       </c>
-      <c r="F53" t="s">
-        <v>17</v>
-      </c>
       <c r="G53" t="s">
+        <v>17</v>
+      </c>
+      <c r="H53" t="s">
         <v>380</v>
       </c>
-      <c r="H53" t="s">
+      <c r="I53" t="s">
         <v>381</v>
       </c>
-      <c r="I53"/>
-      <c r="J53"/>
-      <c r="K53" t="s">
+      <c r="L53" t="s">
         <v>382</v>
       </c>
-      <c r="L53" t="s">
+      <c r="M53" t="s">
         <v>383</v>
       </c>
-      <c r="M53"/>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="O53">
+        <v>2139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4214,33 +4530,39 @@
       <c r="D54" t="s">
         <v>15</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Nov-15 - 9:30 AM</v>
+      </c>
+      <c r="F54" t="s">
         <v>44</v>
       </c>
-      <c r="F54" t="s">
-        <v>17</v>
-      </c>
       <c r="G54" t="s">
+        <v>17</v>
+      </c>
+      <c r="H54" t="s">
         <v>385</v>
       </c>
-      <c r="H54" t="s">
+      <c r="I54" t="s">
         <v>386</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J54" t="s">
         <v>387</v>
       </c>
-      <c r="J54" t="s">
+      <c r="K54" t="s">
         <v>388</v>
       </c>
-      <c r="K54" t="s">
+      <c r="L54" t="s">
         <v>389</v>
       </c>
-      <c r="L54" t="s">
+      <c r="M54" t="s">
         <v>390</v>
       </c>
-      <c r="M54"/>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="O54">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4253,29 +4575,33 @@
       <c r="D55" t="s">
         <v>15</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Nov-16 - 9:30 AM</v>
+      </c>
+      <c r="F55" t="s">
         <v>392</v>
       </c>
-      <c r="F55" t="s">
-        <v>17</v>
-      </c>
       <c r="G55" t="s">
+        <v>17</v>
+      </c>
+      <c r="H55" t="s">
         <v>393</v>
       </c>
-      <c r="H55" t="s">
+      <c r="I55" t="s">
         <v>394</v>
       </c>
-      <c r="I55" t="s">
+      <c r="J55" t="s">
         <v>395</v>
       </c>
-      <c r="J55" t="s">
+      <c r="K55" t="s">
         <v>396</v>
       </c>
-      <c r="K55"/>
-      <c r="L55"/>
-      <c r="M55"/>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="O55">
+        <v>2227</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4288,33 +4614,39 @@
       <c r="D56" t="s">
         <v>15</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Nov-19 - 9:30 AM</v>
+      </c>
+      <c r="F56" t="s">
         <v>398</v>
       </c>
-      <c r="F56" t="s">
-        <v>17</v>
-      </c>
       <c r="G56" t="s">
+        <v>17</v>
+      </c>
+      <c r="H56" t="s">
         <v>399</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I56" t="s">
         <v>400</v>
       </c>
-      <c r="I56" t="s">
+      <c r="J56" t="s">
         <v>401</v>
       </c>
-      <c r="J56" t="s">
+      <c r="K56" t="s">
         <v>402</v>
       </c>
-      <c r="K56" t="s">
+      <c r="L56" t="s">
         <v>403</v>
       </c>
-      <c r="L56" t="s">
+      <c r="M56" t="s">
         <v>404</v>
       </c>
-      <c r="M56"/>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="O56">
+        <v>2274</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4327,33 +4659,39 @@
       <c r="D57" t="s">
         <v>15</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Nov-20 - 9:30 AM</v>
+      </c>
+      <c r="F57" t="s">
         <v>153</v>
       </c>
-      <c r="F57" t="s">
-        <v>17</v>
-      </c>
       <c r="G57" t="s">
+        <v>17</v>
+      </c>
+      <c r="H57" t="s">
         <v>406</v>
       </c>
-      <c r="H57" t="s">
+      <c r="I57" t="s">
         <v>407</v>
       </c>
-      <c r="I57" t="s">
+      <c r="J57" t="s">
         <v>408</v>
       </c>
-      <c r="J57" t="s">
+      <c r="K57" t="s">
         <v>409</v>
       </c>
-      <c r="K57" t="s">
+      <c r="L57" t="s">
         <v>410</v>
       </c>
-      <c r="L57" t="s">
+      <c r="M57" t="s">
         <v>411</v>
       </c>
-      <c r="M57"/>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="O57">
+        <v>2269</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4366,33 +4704,39 @@
       <c r="D58" t="s">
         <v>15</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Nov-21 - 9:30 AM</v>
+      </c>
+      <c r="F58" t="s">
         <v>35</v>
       </c>
-      <c r="F58" t="s">
-        <v>17</v>
-      </c>
       <c r="G58" t="s">
+        <v>17</v>
+      </c>
+      <c r="H58" t="s">
         <v>413</v>
       </c>
-      <c r="H58" t="s">
+      <c r="I58" t="s">
         <v>414</v>
       </c>
-      <c r="I58" t="s">
+      <c r="J58" t="s">
         <v>415</v>
       </c>
-      <c r="J58" t="s">
+      <c r="K58" t="s">
         <v>416</v>
       </c>
-      <c r="K58" t="s">
+      <c r="L58" t="s">
         <v>417</v>
       </c>
-      <c r="L58" t="s">
+      <c r="M58" t="s">
         <v>418</v>
       </c>
-      <c r="M58"/>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="O58">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4405,33 +4749,39 @@
       <c r="D59" t="s">
         <v>15</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Nov-27 - 9:30 AM</v>
+      </c>
+      <c r="F59" t="s">
         <v>420</v>
       </c>
-      <c r="F59" t="s">
-        <v>17</v>
-      </c>
       <c r="G59" t="s">
+        <v>17</v>
+      </c>
+      <c r="H59" t="s">
         <v>421</v>
       </c>
-      <c r="H59" t="s">
+      <c r="I59" t="s">
         <v>422</v>
       </c>
-      <c r="I59" t="s">
+      <c r="J59" t="s">
         <v>423</v>
       </c>
-      <c r="J59" t="s">
+      <c r="K59" t="s">
         <v>424</v>
       </c>
-      <c r="K59" t="s">
+      <c r="L59" t="s">
         <v>425</v>
       </c>
-      <c r="L59" t="s">
+      <c r="M59" t="s">
         <v>426</v>
       </c>
-      <c r="M59"/>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="O59">
+        <v>2281</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4444,29 +4794,33 @@
       <c r="D60" t="s">
         <v>116</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Nov-28 - 10:00 AM</v>
+      </c>
+      <c r="F60" t="s">
         <v>249</v>
       </c>
-      <c r="F60" t="s">
-        <v>17</v>
-      </c>
       <c r="G60" t="s">
+        <v>17</v>
+      </c>
+      <c r="H60" t="s">
         <v>428</v>
       </c>
-      <c r="H60" t="s">
+      <c r="I60" t="s">
         <v>429</v>
       </c>
-      <c r="I60"/>
-      <c r="J60"/>
-      <c r="K60" t="s">
+      <c r="L60" t="s">
         <v>430</v>
       </c>
-      <c r="L60" t="s">
+      <c r="M60" t="s">
         <v>431</v>
       </c>
-      <c r="M60"/>
-    </row>
-    <row r="61" spans="1:13">
+      <c r="O60">
+        <v>2413</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4479,29 +4833,33 @@
       <c r="D61" t="s">
         <v>433</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Nov-29 - 1:30 PM</v>
+      </c>
+      <c r="F61" t="s">
         <v>100</v>
       </c>
-      <c r="F61" t="s">
-        <v>17</v>
-      </c>
       <c r="G61" t="s">
+        <v>17</v>
+      </c>
+      <c r="H61" t="s">
         <v>434</v>
       </c>
-      <c r="H61" t="s">
+      <c r="I61" t="s">
         <v>435</v>
       </c>
-      <c r="I61" t="s">
+      <c r="J61" t="s">
         <v>436</v>
       </c>
-      <c r="J61" t="s">
+      <c r="K61" t="s">
         <v>437</v>
       </c>
-      <c r="K61"/>
-      <c r="L61"/>
-      <c r="M61"/>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="O61">
+        <v>2226</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4514,33 +4872,39 @@
       <c r="D62" t="s">
         <v>15</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Dec-04 - 9:30 AM</v>
+      </c>
+      <c r="F62" t="s">
         <v>83</v>
       </c>
-      <c r="F62" t="s">
-        <v>17</v>
-      </c>
       <c r="G62" t="s">
+        <v>17</v>
+      </c>
+      <c r="H62" t="s">
         <v>439</v>
       </c>
-      <c r="H62" t="s">
+      <c r="I62" t="s">
         <v>440</v>
       </c>
-      <c r="I62" t="s">
+      <c r="J62" t="s">
         <v>441</v>
       </c>
-      <c r="J62" t="s">
+      <c r="K62" t="s">
         <v>442</v>
       </c>
-      <c r="K62" t="s">
+      <c r="L62" t="s">
         <v>443</v>
       </c>
-      <c r="L62" t="s">
+      <c r="M62" t="s">
         <v>444</v>
       </c>
-      <c r="M62"/>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="O62">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4553,33 +4917,39 @@
       <c r="D63" t="s">
         <v>446</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Dec-05 - 12:00 PM</v>
+      </c>
+      <c r="F63" t="s">
         <v>447</v>
       </c>
-      <c r="F63" t="s">
-        <v>17</v>
-      </c>
       <c r="G63" t="s">
+        <v>17</v>
+      </c>
+      <c r="H63" t="s">
         <v>448</v>
       </c>
-      <c r="H63" t="s">
+      <c r="I63" t="s">
         <v>449</v>
       </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
         <v>450</v>
       </c>
-      <c r="J63" t="s">
+      <c r="K63" t="s">
         <v>451</v>
       </c>
-      <c r="K63" t="s">
+      <c r="L63" t="s">
         <v>452</v>
       </c>
-      <c r="L63" t="s">
+      <c r="M63" t="s">
         <v>453</v>
       </c>
-      <c r="M63"/>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="O63">
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4592,33 +4962,39 @@
       <c r="D64" t="s">
         <v>15</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Dec-06 - 9:30 AM</v>
+      </c>
+      <c r="F64" t="s">
         <v>455</v>
       </c>
-      <c r="F64" t="s">
-        <v>17</v>
-      </c>
       <c r="G64" t="s">
+        <v>17</v>
+      </c>
+      <c r="H64" t="s">
         <v>456</v>
       </c>
-      <c r="H64" t="s">
+      <c r="I64" t="s">
         <v>457</v>
       </c>
-      <c r="I64" t="s">
+      <c r="J64" t="s">
         <v>458</v>
       </c>
-      <c r="J64" t="s">
+      <c r="K64" t="s">
         <v>459</v>
       </c>
-      <c r="K64" t="s">
+      <c r="L64" t="s">
         <v>460</v>
       </c>
-      <c r="L64" t="s">
+      <c r="M64" t="s">
         <v>461</v>
       </c>
-      <c r="M64"/>
-    </row>
-    <row r="65" spans="1:13">
+      <c r="O64">
+        <v>2279</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4631,33 +5007,39 @@
       <c r="D65" t="s">
         <v>463</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Dec-10 - 1:00 PM</v>
+      </c>
+      <c r="F65" t="s">
         <v>16</v>
       </c>
-      <c r="F65" t="s">
-        <v>17</v>
-      </c>
       <c r="G65" t="s">
+        <v>17</v>
+      </c>
+      <c r="H65" t="s">
         <v>464</v>
       </c>
-      <c r="H65" t="s">
+      <c r="I65" t="s">
         <v>465</v>
       </c>
-      <c r="I65" t="s">
+      <c r="J65" t="s">
         <v>466</v>
       </c>
-      <c r="J65" t="s">
+      <c r="K65" t="s">
         <v>467</v>
       </c>
-      <c r="K65" t="s">
+      <c r="L65" t="s">
         <v>468</v>
       </c>
-      <c r="L65" t="s">
+      <c r="M65" t="s">
         <v>469</v>
       </c>
-      <c r="M65"/>
-    </row>
-    <row r="66" spans="1:13">
+      <c r="O65">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4670,33 +5052,39 @@
       <c r="D66" t="s">
         <v>15</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" t="str">
+        <f t="shared" si="0"/>
+        <v>2012-Dec-11 - 9:30 AM</v>
+      </c>
+      <c r="F66" t="s">
         <v>130</v>
       </c>
-      <c r="F66" t="s">
-        <v>17</v>
-      </c>
       <c r="G66" t="s">
+        <v>17</v>
+      </c>
+      <c r="H66" t="s">
         <v>471</v>
       </c>
-      <c r="H66" t="s">
+      <c r="I66" t="s">
         <v>472</v>
       </c>
-      <c r="I66" t="s">
+      <c r="J66" t="s">
         <v>473</v>
       </c>
-      <c r="J66" t="s">
+      <c r="K66" t="s">
         <v>474</v>
       </c>
-      <c r="K66" t="s">
+      <c r="L66" t="s">
         <v>475</v>
       </c>
-      <c r="L66" t="s">
+      <c r="M66" t="s">
         <v>476</v>
       </c>
-      <c r="M66"/>
-    </row>
-    <row r="67" spans="1:13">
+      <c r="O66">
+        <v>2282</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4709,29 +5097,33 @@
       <c r="D67" t="s">
         <v>116</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" t="str">
+        <f t="shared" ref="E67:E87" si="1">C67&amp;" - "&amp;D67</f>
+        <v>2012-Dec-12 - 10:00 AM</v>
+      </c>
+      <c r="F67" t="s">
         <v>478</v>
       </c>
-      <c r="F67" t="s">
-        <v>17</v>
-      </c>
       <c r="G67" t="s">
+        <v>17</v>
+      </c>
+      <c r="H67" t="s">
         <v>479</v>
       </c>
-      <c r="H67" t="s">
+      <c r="I67" t="s">
         <v>480</v>
       </c>
-      <c r="I67"/>
-      <c r="J67"/>
-      <c r="K67" t="s">
+      <c r="L67" t="s">
         <v>481</v>
       </c>
-      <c r="L67" t="s">
+      <c r="M67" t="s">
         <v>482</v>
       </c>
-      <c r="M67"/>
-    </row>
-    <row r="68" spans="1:13">
+      <c r="O67">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4744,25 +5136,27 @@
       <c r="D68" t="s">
         <v>116</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" t="str">
+        <f t="shared" si="1"/>
+        <v>2012-Dec-13 - 10:00 AM</v>
+      </c>
+      <c r="F68" t="s">
         <v>249</v>
       </c>
-      <c r="F68" t="s">
-        <v>17</v>
-      </c>
       <c r="G68" t="s">
+        <v>17</v>
+      </c>
+      <c r="H68" t="s">
         <v>485</v>
       </c>
-      <c r="H68" t="s">
+      <c r="I68" t="s">
         <v>486</v>
       </c>
-      <c r="I68"/>
-      <c r="J68"/>
-      <c r="K68"/>
-      <c r="L68"/>
-      <c r="M68"/>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="O68">
+        <v>2446</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4775,29 +5169,33 @@
       <c r="D69" t="s">
         <v>116</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" t="str">
+        <f t="shared" si="1"/>
+        <v>2012-Dec-19 - 10:00 AM</v>
+      </c>
+      <c r="F69" t="s">
         <v>249</v>
       </c>
-      <c r="F69" t="s">
-        <v>17</v>
-      </c>
       <c r="G69" t="s">
+        <v>17</v>
+      </c>
+      <c r="H69" t="s">
         <v>488</v>
       </c>
-      <c r="H69" t="s">
+      <c r="I69" t="s">
         <v>489</v>
       </c>
-      <c r="I69"/>
-      <c r="J69"/>
-      <c r="K69" t="s">
+      <c r="L69" t="s">
         <v>490</v>
       </c>
-      <c r="L69" t="s">
+      <c r="M69" t="s">
         <v>491</v>
       </c>
-      <c r="M69"/>
-    </row>
-    <row r="70" spans="1:13">
+      <c r="O69">
+        <v>2439</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4810,25 +5208,27 @@
       <c r="D70" t="s">
         <v>116</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Jan-09 - 10:00 AM</v>
+      </c>
+      <c r="F70" t="s">
         <v>494</v>
       </c>
-      <c r="F70" t="s">
-        <v>17</v>
-      </c>
       <c r="G70" t="s">
+        <v>17</v>
+      </c>
+      <c r="H70" t="s">
         <v>495</v>
       </c>
-      <c r="H70" t="s">
+      <c r="I70" t="s">
         <v>496</v>
       </c>
-      <c r="I70"/>
-      <c r="J70"/>
-      <c r="K70"/>
-      <c r="L70"/>
-      <c r="M70"/>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="O70">
+        <v>2483</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4841,33 +5241,39 @@
       <c r="D71" t="s">
         <v>15</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Jan-14 - 9:30 AM</v>
+      </c>
+      <c r="F71" t="s">
         <v>498</v>
       </c>
-      <c r="F71" t="s">
-        <v>17</v>
-      </c>
       <c r="G71" t="s">
+        <v>17</v>
+      </c>
+      <c r="H71" t="s">
         <v>499</v>
       </c>
-      <c r="H71" t="s">
+      <c r="I71" t="s">
         <v>500</v>
       </c>
-      <c r="I71" t="s">
+      <c r="J71" t="s">
         <v>501</v>
       </c>
-      <c r="J71" t="s">
+      <c r="K71" t="s">
         <v>502</v>
       </c>
-      <c r="K71" t="s">
+      <c r="L71" t="s">
         <v>503</v>
       </c>
-      <c r="L71" t="s">
+      <c r="M71" t="s">
         <v>504</v>
       </c>
-      <c r="M71"/>
-    </row>
-    <row r="72" spans="1:13">
+      <c r="O71">
+        <v>2406</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4880,33 +5286,39 @@
       <c r="D72" t="s">
         <v>15</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Jan-15 - 9:30 AM</v>
+      </c>
+      <c r="F72" t="s">
         <v>506</v>
       </c>
-      <c r="F72" t="s">
-        <v>17</v>
-      </c>
       <c r="G72" t="s">
+        <v>17</v>
+      </c>
+      <c r="H72" t="s">
         <v>507</v>
       </c>
-      <c r="H72" t="s">
+      <c r="I72" t="s">
         <v>508</v>
       </c>
-      <c r="I72" t="s">
+      <c r="J72" t="s">
         <v>509</v>
       </c>
-      <c r="J72" t="s">
+      <c r="K72" t="s">
         <v>510</v>
       </c>
-      <c r="K72" t="s">
+      <c r="L72" t="s">
         <v>511</v>
       </c>
-      <c r="L72" t="s">
+      <c r="M72" t="s">
         <v>512</v>
       </c>
-      <c r="M72"/>
-    </row>
-    <row r="73" spans="1:13">
+      <c r="O72">
+        <v>2292</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4919,33 +5331,39 @@
       <c r="D73" t="s">
         <v>15</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Jan-16 - 9:30 AM</v>
+      </c>
+      <c r="F73" t="s">
         <v>514</v>
       </c>
-      <c r="F73" t="s">
-        <v>17</v>
-      </c>
       <c r="G73" t="s">
+        <v>17</v>
+      </c>
+      <c r="H73" t="s">
         <v>515</v>
       </c>
-      <c r="H73" t="s">
+      <c r="I73" t="s">
         <v>516</v>
       </c>
-      <c r="I73" t="s">
+      <c r="J73" t="s">
         <v>517</v>
       </c>
-      <c r="J73" t="s">
+      <c r="K73" t="s">
         <v>518</v>
       </c>
-      <c r="K73" t="s">
+      <c r="L73" t="s">
         <v>519</v>
       </c>
-      <c r="L73" t="s">
+      <c r="M73" t="s">
         <v>520</v>
       </c>
-      <c r="M73"/>
-    </row>
-    <row r="74" spans="1:13">
+      <c r="O73">
+        <v>2271</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4958,33 +5376,39 @@
       <c r="D74" t="s">
         <v>15</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Jan-17 - 9:30 AM</v>
+      </c>
+      <c r="F74" t="s">
         <v>392</v>
       </c>
-      <c r="F74" t="s">
-        <v>17</v>
-      </c>
       <c r="G74" t="s">
+        <v>17</v>
+      </c>
+      <c r="H74" t="s">
         <v>522</v>
       </c>
-      <c r="H74" t="s">
+      <c r="I74" t="s">
         <v>523</v>
       </c>
-      <c r="I74" t="s">
+      <c r="J74" t="s">
         <v>524</v>
       </c>
-      <c r="J74" t="s">
+      <c r="K74" t="s">
         <v>525</v>
       </c>
-      <c r="K74" t="s">
+      <c r="L74" t="s">
         <v>526</v>
       </c>
-      <c r="L74" t="s">
+      <c r="M74" t="s">
         <v>527</v>
       </c>
-      <c r="M74"/>
-    </row>
-    <row r="75" spans="1:13">
+      <c r="O74">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4997,29 +5421,33 @@
       <c r="D75" t="s">
         <v>433</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Jan-17 - 1:30 PM</v>
+      </c>
+      <c r="F75" t="s">
         <v>44</v>
       </c>
-      <c r="F75" t="s">
-        <v>17</v>
-      </c>
       <c r="G75" t="s">
+        <v>17</v>
+      </c>
+      <c r="H75" t="s">
         <v>528</v>
       </c>
-      <c r="H75" t="s">
+      <c r="I75" t="s">
         <v>529</v>
       </c>
-      <c r="I75" t="s">
+      <c r="J75" t="s">
         <v>530</v>
       </c>
-      <c r="J75" t="s">
+      <c r="K75" t="s">
         <v>531</v>
       </c>
-      <c r="K75"/>
-      <c r="L75"/>
-      <c r="M75"/>
-    </row>
-    <row r="76" spans="1:13">
+      <c r="O75">
+        <v>2431</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
       <c r="A76">
         <v>75</v>
       </c>
@@ -5032,25 +5460,27 @@
       <c r="D76" t="s">
         <v>123</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Jan-17 - 6:00 PM</v>
+      </c>
+      <c r="F76" t="s">
         <v>532</v>
       </c>
-      <c r="F76" t="s">
-        <v>17</v>
-      </c>
       <c r="G76" t="s">
+        <v>17</v>
+      </c>
+      <c r="H76" t="s">
         <v>533</v>
       </c>
-      <c r="H76" t="s">
+      <c r="I76" t="s">
         <v>534</v>
       </c>
-      <c r="I76"/>
-      <c r="J76"/>
-      <c r="K76"/>
-      <c r="L76"/>
-      <c r="M76"/>
-    </row>
-    <row r="77" spans="1:13">
+      <c r="O76">
+        <v>2452</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15">
       <c r="A77">
         <v>76</v>
       </c>
@@ -5063,33 +5493,39 @@
       <c r="D77" t="s">
         <v>15</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Jan-21 - 9:30 AM</v>
+      </c>
+      <c r="F77" t="s">
         <v>83</v>
       </c>
-      <c r="F77" t="s">
-        <v>17</v>
-      </c>
       <c r="G77" t="s">
+        <v>17</v>
+      </c>
+      <c r="H77" t="s">
         <v>536</v>
       </c>
-      <c r="H77" t="s">
+      <c r="I77" t="s">
         <v>537</v>
       </c>
-      <c r="I77" t="s">
+      <c r="J77" t="s">
         <v>538</v>
       </c>
-      <c r="J77" t="s">
+      <c r="K77" t="s">
         <v>539</v>
       </c>
-      <c r="K77" t="s">
+      <c r="L77" t="s">
         <v>540</v>
       </c>
-      <c r="L77" t="s">
+      <c r="M77" t="s">
         <v>541</v>
       </c>
-      <c r="M77"/>
-    </row>
-    <row r="78" spans="1:13">
+      <c r="O77">
+        <v>2424</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
       <c r="A78">
         <v>77</v>
       </c>
@@ -5102,31 +5538,36 @@
       <c r="D78" t="s">
         <v>116</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Jan-23 - 10:00 AM</v>
+      </c>
+      <c r="F78" t="s">
         <v>249</v>
       </c>
-      <c r="F78" t="s">
-        <v>17</v>
-      </c>
       <c r="G78" t="s">
+        <v>17</v>
+      </c>
+      <c r="H78" t="s">
         <v>543</v>
       </c>
-      <c r="H78" t="s">
+      <c r="I78" t="s">
         <v>544</v>
       </c>
-      <c r="I78"/>
-      <c r="J78"/>
-      <c r="K78" t="s">
+      <c r="L78" t="s">
         <v>545</v>
       </c>
-      <c r="L78" t="s">
+      <c r="M78" t="s">
         <v>546</v>
       </c>
-      <c r="M78" t="s">
+      <c r="N78" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="79" spans="1:13">
+      <c r="O78">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5139,25 +5580,27 @@
       <c r="D79" t="s">
         <v>116</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Jan-30 - 10:00 AM</v>
+      </c>
+      <c r="F79" t="s">
         <v>550</v>
       </c>
-      <c r="F79" t="s">
-        <v>17</v>
-      </c>
       <c r="G79" t="s">
+        <v>17</v>
+      </c>
+      <c r="H79" t="s">
         <v>551</v>
       </c>
-      <c r="H79" t="s">
+      <c r="I79" t="s">
         <v>552</v>
       </c>
-      <c r="I79"/>
-      <c r="J79"/>
-      <c r="K79"/>
-      <c r="L79"/>
-      <c r="M79"/>
-    </row>
-    <row r="80" spans="1:13">
+      <c r="O79">
+        <v>2486</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5170,31 +5613,36 @@
       <c r="D80" t="s">
         <v>15</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Feb-05 - 9:30 AM</v>
+      </c>
+      <c r="F80" t="s">
         <v>83</v>
       </c>
-      <c r="F80" t="s">
-        <v>17</v>
-      </c>
       <c r="G80" t="s">
+        <v>17</v>
+      </c>
+      <c r="H80" t="s">
         <v>554</v>
       </c>
-      <c r="H80" t="s">
+      <c r="I80" t="s">
         <v>555</v>
       </c>
-      <c r="I80" t="s">
+      <c r="J80" t="s">
         <v>556</v>
       </c>
-      <c r="J80" t="s">
+      <c r="K80" t="s">
         <v>557</v>
       </c>
-      <c r="K80"/>
-      <c r="L80"/>
-      <c r="M80" t="s">
+      <c r="N80" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="81" spans="1:13">
+      <c r="O80">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15">
       <c r="A81">
         <v>80</v>
       </c>
@@ -5207,31 +5655,36 @@
       <c r="D81" t="s">
         <v>15</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Feb-06 - 9:30 AM</v>
+      </c>
+      <c r="F81" t="s">
         <v>559</v>
       </c>
-      <c r="F81" t="s">
-        <v>17</v>
-      </c>
       <c r="G81" t="s">
+        <v>17</v>
+      </c>
+      <c r="H81" t="s">
         <v>560</v>
       </c>
-      <c r="H81" t="s">
+      <c r="I81" t="s">
         <v>561</v>
       </c>
-      <c r="I81" t="s">
+      <c r="J81" t="s">
         <v>562</v>
       </c>
-      <c r="J81" t="s">
+      <c r="K81" t="s">
         <v>563</v>
       </c>
-      <c r="K81"/>
-      <c r="L81"/>
-      <c r="M81" t="s">
+      <c r="N81" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="82" spans="1:13">
+      <c r="O81">
+        <v>2233</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5244,31 +5697,36 @@
       <c r="D82" t="s">
         <v>15</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Feb-07 - 9:30 AM</v>
+      </c>
+      <c r="F82" t="s">
         <v>565</v>
       </c>
-      <c r="F82" t="s">
-        <v>17</v>
-      </c>
       <c r="G82" t="s">
+        <v>17</v>
+      </c>
+      <c r="H82" t="s">
         <v>566</v>
       </c>
-      <c r="H82" t="s">
+      <c r="I82" t="s">
         <v>567</v>
       </c>
-      <c r="I82" t="s">
+      <c r="J82" t="s">
         <v>568</v>
       </c>
-      <c r="J82" t="s">
+      <c r="K82" t="s">
         <v>569</v>
       </c>
-      <c r="K82"/>
-      <c r="L82"/>
-      <c r="M82" t="s">
+      <c r="N82" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="83" spans="1:13">
+      <c r="O82">
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5281,31 +5739,36 @@
       <c r="D83" t="s">
         <v>15</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Feb-12 - 9:30 AM</v>
+      </c>
+      <c r="F83" t="s">
         <v>571</v>
       </c>
-      <c r="F83" t="s">
-        <v>17</v>
-      </c>
       <c r="G83" t="s">
+        <v>17</v>
+      </c>
+      <c r="H83" t="s">
         <v>572</v>
       </c>
-      <c r="H83" t="s">
+      <c r="I83" t="s">
         <v>573</v>
       </c>
-      <c r="I83" t="s">
+      <c r="J83" t="s">
         <v>574</v>
       </c>
-      <c r="J83" t="s">
+      <c r="K83" t="s">
         <v>575</v>
       </c>
-      <c r="K83"/>
-      <c r="L83"/>
-      <c r="M83" t="s">
+      <c r="N83" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="84" spans="1:13">
+      <c r="O83">
+        <v>2326</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5318,31 +5781,36 @@
       <c r="D84" t="s">
         <v>116</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Feb-13 - 10:00 AM</v>
+      </c>
+      <c r="F84" t="s">
         <v>249</v>
       </c>
-      <c r="F84" t="s">
-        <v>17</v>
-      </c>
       <c r="G84" t="s">
+        <v>17</v>
+      </c>
+      <c r="H84" t="s">
         <v>577</v>
       </c>
-      <c r="H84" t="s">
+      <c r="I84" t="s">
         <v>578</v>
       </c>
-      <c r="I84" t="s">
+      <c r="J84" t="s">
         <v>579</v>
       </c>
-      <c r="J84" t="s">
+      <c r="K84" t="s">
         <v>580</v>
       </c>
-      <c r="K84"/>
-      <c r="L84"/>
-      <c r="M84" t="s">
+      <c r="N84" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="85" spans="1:13">
+      <c r="O84">
+        <v>2479</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5355,31 +5823,36 @@
       <c r="D85" t="s">
         <v>15</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Feb-19 - 9:30 AM</v>
+      </c>
+      <c r="F85" t="s">
         <v>582</v>
       </c>
-      <c r="F85" t="s">
-        <v>17</v>
-      </c>
       <c r="G85" t="s">
+        <v>17</v>
+      </c>
+      <c r="H85" t="s">
         <v>583</v>
       </c>
-      <c r="H85" t="s">
+      <c r="I85" t="s">
         <v>584</v>
       </c>
-      <c r="I85" t="s">
+      <c r="J85" t="s">
         <v>585</v>
       </c>
-      <c r="J85" t="s">
+      <c r="K85" t="s">
         <v>586</v>
       </c>
-      <c r="K85"/>
-      <c r="L85"/>
-      <c r="M85" t="s">
+      <c r="N85" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="86" spans="1:13">
+      <c r="O85">
+        <v>2398</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5392,31 +5865,36 @@
       <c r="D86" t="s">
         <v>15</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Feb-20 - 9:30 AM</v>
+      </c>
+      <c r="F86" t="s">
         <v>514</v>
       </c>
-      <c r="F86" t="s">
-        <v>17</v>
-      </c>
       <c r="G86" t="s">
+        <v>17</v>
+      </c>
+      <c r="H86" t="s">
         <v>588</v>
       </c>
-      <c r="H86" t="s">
+      <c r="I86" t="s">
         <v>589</v>
       </c>
-      <c r="I86" t="s">
+      <c r="J86" t="s">
         <v>590</v>
       </c>
-      <c r="J86" t="s">
+      <c r="K86" t="s">
         <v>591</v>
       </c>
-      <c r="K86"/>
-      <c r="L86"/>
-      <c r="M86" t="s">
+      <c r="N86" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="87" spans="1:13">
+      <c r="O86">
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5429,40 +5907,40 @@
       <c r="D87" t="s">
         <v>15</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" t="str">
+        <f t="shared" si="1"/>
+        <v>2013-Feb-21 - 9:30 AM</v>
+      </c>
+      <c r="F87" t="s">
         <v>44</v>
       </c>
-      <c r="F87" t="s">
-        <v>17</v>
-      </c>
       <c r="G87" t="s">
+        <v>17</v>
+      </c>
+      <c r="H87" t="s">
         <v>593</v>
       </c>
-      <c r="H87" t="s">
+      <c r="I87" t="s">
         <v>594</v>
       </c>
-      <c r="I87" t="s">
+      <c r="J87" t="s">
         <v>595</v>
       </c>
-      <c r="J87" t="s">
+      <c r="K87" t="s">
         <v>596</v>
       </c>
-      <c r="K87"/>
-      <c r="L87"/>
-      <c r="M87"/>
+      <c r="O87">
+        <v>2333</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with UnixDateTime Column
</commit_message>
<xml_diff>
--- a/Excel File Manual Tests/SearchResultsTable.xlsx
+++ b/Excel File Manual Tests/SearchResultsTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23117"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="2300" windowWidth="25600" windowHeight="14980"/>
+    <workbookView xWindow="1560" yWindow="1180" windowWidth="25600" windowHeight="14980"/>
   </bookViews>
   <sheets>
     <sheet name="SearchResultsTable" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="600">
   <si>
     <t>id</t>
   </si>
@@ -1855,6 +1855,9 @@
   </si>
   <si>
     <t>MeetID</t>
+  </si>
+  <si>
+    <t>UnixDateTime</t>
   </si>
 </sst>
 </file>
@@ -1897,7 +1900,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1907,19 +1910,92 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2212,15 +2288,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O87"/>
+  <dimension ref="A1:P87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="30.1640625" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2266,8 +2346,11 @@
       <c r="O1" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2280,9 +2363,8 @@
       <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="str">
-        <f>C2&amp;" - "&amp;D2</f>
-        <v>2012-Jun-18 - 9:30 AM</v>
+      <c r="E2" s="1">
+        <v>41078.395833333336</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -2311,8 +2393,12 @@
       <c r="O2">
         <v>1927</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2">
+        <f xml:space="preserve"> (E2 * 86400) - 2209075200</f>
+        <v>1340098200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2325,9 +2411,8 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" si="0">C3&amp;" - "&amp;D3</f>
-        <v>2012-Jun-19 - 9:30 AM</v>
+      <c r="E3" s="1">
+        <v>41079.395833333336</v>
       </c>
       <c r="F3" t="s">
         <v>26</v>
@@ -2356,8 +2441,12 @@
       <c r="O3">
         <v>2407</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3">
+        <f t="shared" ref="P3:P66" si="0" xml:space="preserve"> (E3 * 86400) - 2209075200</f>
+        <v>1340184600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2370,9 +2459,8 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Jun-20 - 9:30 AM</v>
+      <c r="E4" s="1">
+        <v>41080.395833333336</v>
       </c>
       <c r="F4" t="s">
         <v>35</v>
@@ -2401,8 +2489,12 @@
       <c r="O4">
         <v>2147</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>1340271000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2415,9 +2507,8 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Jun-21 - 9:30 AM</v>
+      <c r="E5" s="1">
+        <v>41081.395833333336</v>
       </c>
       <c r="F5" t="s">
         <v>44</v>
@@ -2446,8 +2537,12 @@
       <c r="O5">
         <v>2154</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>1340357400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2460,9 +2555,8 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Jun-21 - 9:30 AM</v>
+      <c r="E6" s="1">
+        <v>41081.395833333336</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>
@@ -2485,8 +2579,12 @@
       <c r="O6">
         <v>2409</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>1340357400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2499,9 +2597,8 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Jun-25 - 9:30 AM</v>
+      <c r="E7" s="1">
+        <v>41085.395833333336</v>
       </c>
       <c r="F7" t="s">
         <v>58</v>
@@ -2530,8 +2627,12 @@
       <c r="O7">
         <v>2211</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>1340703000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2544,9 +2645,8 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Jun-26 - 9:30 AM</v>
+      <c r="E8" s="1">
+        <v>41086.395833333336</v>
       </c>
       <c r="F8" t="s">
         <v>67</v>
@@ -2575,8 +2675,12 @@
       <c r="O8">
         <v>2181</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>1340789400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2589,9 +2693,8 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Jun-27 - 9:30 AM</v>
+      <c r="E9" s="1">
+        <v>41087.395833333336</v>
       </c>
       <c r="F9" t="s">
         <v>76</v>
@@ -2614,8 +2717,12 @@
       <c r="O9">
         <v>2484</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>1340875800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2628,9 +2735,8 @@
       <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Jul-03 - 9:30 AM</v>
+      <c r="E10" s="1">
+        <v>41093.395833333336</v>
       </c>
       <c r="F10" t="s">
         <v>83</v>
@@ -2659,8 +2765,12 @@
       <c r="O10">
         <v>2412</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>1341394200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2673,9 +2783,8 @@
       <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Jul-04 - 9:30 AM</v>
+      <c r="E11" s="1">
+        <v>41094.395833333336</v>
       </c>
       <c r="F11" t="s">
         <v>92</v>
@@ -2704,8 +2813,12 @@
       <c r="O11">
         <v>2411</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>1341480600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2718,9 +2831,8 @@
       <c r="D12" t="s">
         <v>15</v>
       </c>
-      <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Jul-06 - 9:30 AM</v>
+      <c r="E12" s="1">
+        <v>41096.395833333336</v>
       </c>
       <c r="F12" t="s">
         <v>100</v>
@@ -2749,8 +2861,12 @@
       <c r="O12">
         <v>2216</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>1341653400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2763,9 +2879,8 @@
       <c r="D13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Jul-09 - 9:30 AM</v>
+      <c r="E13" s="1">
+        <v>41099.395833333336</v>
       </c>
       <c r="F13" t="s">
         <v>108</v>
@@ -2794,8 +2909,12 @@
       <c r="O13">
         <v>2362</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>1341912600</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2808,9 +2927,8 @@
       <c r="D14" t="s">
         <v>116</v>
       </c>
-      <c r="E14" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Jul-11 - 10:00 AM</v>
+      <c r="E14" s="1">
+        <v>41101.416666666664</v>
       </c>
       <c r="F14" t="s">
         <v>117</v>
@@ -2833,8 +2951,12 @@
       <c r="O14">
         <v>2487</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>1342087200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2847,9 +2969,8 @@
       <c r="D15" t="s">
         <v>123</v>
       </c>
-      <c r="E15" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Aug-02 - 6:00 PM</v>
+      <c r="E15" s="1">
+        <v>41123.75</v>
       </c>
       <c r="F15" t="s">
         <v>124</v>
@@ -2872,8 +2993,12 @@
       <c r="O15">
         <v>2410</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>1344016800</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2886,9 +3011,8 @@
       <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="E16" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Aug-23 - 9:30 AM</v>
+      <c r="E16" s="1">
+        <v>41144.395833333336</v>
       </c>
       <c r="F16" t="s">
         <v>130</v>
@@ -2917,8 +3041,12 @@
       <c r="O16">
         <v>2361</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>1345800600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2931,9 +3059,8 @@
       <c r="D17" t="s">
         <v>15</v>
       </c>
-      <c r="E17" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Aug-24 - 9:30 AM</v>
+      <c r="E17" s="1">
+        <v>41145.395833333336</v>
       </c>
       <c r="F17" t="s">
         <v>138</v>
@@ -2962,8 +3089,12 @@
       <c r="O17">
         <v>2214</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="P17">
+        <f t="shared" si="0"/>
+        <v>1345887000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2976,9 +3107,8 @@
       <c r="D18" t="s">
         <v>15</v>
       </c>
-      <c r="E18" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Aug-27 - 9:30 AM</v>
+      <c r="E18" s="1">
+        <v>41148.395833333336</v>
       </c>
       <c r="F18" t="s">
         <v>100</v>
@@ -3007,8 +3137,12 @@
       <c r="O18">
         <v>2143</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="P18">
+        <f t="shared" si="0"/>
+        <v>1346146200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3021,9 +3155,8 @@
       <c r="D19" t="s">
         <v>15</v>
       </c>
-      <c r="E19" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Aug-28 - 9:30 AM</v>
+      <c r="E19" s="1">
+        <v>41149.395833333336</v>
       </c>
       <c r="F19" t="s">
         <v>153</v>
@@ -3052,8 +3185,12 @@
       <c r="O19">
         <v>2213</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="P19">
+        <f t="shared" si="0"/>
+        <v>1346232600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3066,9 +3203,8 @@
       <c r="D20" t="s">
         <v>116</v>
       </c>
-      <c r="E20" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Aug-28 - 10:00 AM</v>
+      <c r="E20" s="1">
+        <v>41149.416666666664</v>
       </c>
       <c r="F20" t="s">
         <v>161</v>
@@ -3085,8 +3221,12 @@
       <c r="O20">
         <v>2221</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="P20">
+        <f t="shared" si="0"/>
+        <v>1346234400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3099,9 +3239,8 @@
       <c r="D21" t="s">
         <v>116</v>
       </c>
-      <c r="E21" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Aug-29 - 10:00 AM</v>
+      <c r="E21" s="1">
+        <v>41150.416666666664</v>
       </c>
       <c r="F21" t="s">
         <v>165</v>
@@ -3124,8 +3263,12 @@
       <c r="O21">
         <v>2151</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="P21">
+        <f t="shared" si="0"/>
+        <v>1346320800</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3138,9 +3281,8 @@
       <c r="D22" t="s">
         <v>15</v>
       </c>
-      <c r="E22" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Aug-30 - 9:30 AM</v>
+      <c r="E22" s="1">
+        <v>41151.395833333336</v>
       </c>
       <c r="F22" t="s">
         <v>171</v>
@@ -3169,8 +3311,12 @@
       <c r="O22">
         <v>2219</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="P22">
+        <f t="shared" si="0"/>
+        <v>1346405400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3183,9 +3329,8 @@
       <c r="D23" t="s">
         <v>15</v>
       </c>
-      <c r="E23" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Sep-05 - 9:30 AM</v>
+      <c r="E23" s="1">
+        <v>41157.395833333336</v>
       </c>
       <c r="F23" t="s">
         <v>16</v>
@@ -3214,8 +3359,12 @@
       <c r="O23">
         <v>2121</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="P23">
+        <f t="shared" si="0"/>
+        <v>1346923800</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3228,9 +3377,8 @@
       <c r="D24" t="s">
         <v>15</v>
       </c>
-      <c r="E24" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Sep-06 - 9:30 AM</v>
+      <c r="E24" s="1">
+        <v>41158.395833333336</v>
       </c>
       <c r="F24" t="s">
         <v>44</v>
@@ -3259,8 +3407,12 @@
       <c r="O24">
         <v>2364</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="P24">
+        <f t="shared" si="0"/>
+        <v>1347010200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3273,9 +3425,8 @@
       <c r="D25" t="s">
         <v>15</v>
       </c>
-      <c r="E25" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Sep-11 - 9:30 AM</v>
+      <c r="E25" s="1">
+        <v>41163.395833333336</v>
       </c>
       <c r="F25" t="s">
         <v>108</v>
@@ -3304,8 +3455,12 @@
       <c r="O25">
         <v>2360</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="P25">
+        <f t="shared" si="0"/>
+        <v>1347442200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3318,9 +3473,8 @@
       <c r="D26" t="s">
         <v>15</v>
       </c>
-      <c r="E26" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Sep-12 - 9:30 AM</v>
+      <c r="E26" s="1">
+        <v>41164.395833333336</v>
       </c>
       <c r="F26" t="s">
         <v>200</v>
@@ -3349,8 +3503,12 @@
       <c r="O26">
         <v>2408</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="P26">
+        <f t="shared" si="0"/>
+        <v>1347528600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3363,9 +3521,8 @@
       <c r="D27" t="s">
         <v>15</v>
       </c>
-      <c r="E27" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Sep-13 - 9:30 AM</v>
+      <c r="E27" s="1">
+        <v>41165.395833333336</v>
       </c>
       <c r="F27" t="s">
         <v>100</v>
@@ -3394,8 +3551,12 @@
       <c r="O27">
         <v>2204</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="P27">
+        <f t="shared" si="0"/>
+        <v>1347615000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3408,9 +3569,8 @@
       <c r="D28" t="s">
         <v>15</v>
       </c>
-      <c r="E28" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Sep-17 - 9:30 AM</v>
+      <c r="E28" s="1">
+        <v>41169.395833333336</v>
       </c>
       <c r="F28" t="s">
         <v>216</v>
@@ -3439,8 +3599,12 @@
       <c r="O28">
         <v>2275</v>
       </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="P28">
+        <f t="shared" si="0"/>
+        <v>1347960600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3453,9 +3617,8 @@
       <c r="D29" t="s">
         <v>15</v>
       </c>
-      <c r="E29" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Sep-19 - 9:30 AM</v>
+      <c r="E29" s="1">
+        <v>41171.395833333336</v>
       </c>
       <c r="F29" t="s">
         <v>100</v>
@@ -3484,8 +3647,12 @@
       <c r="O29">
         <v>2224</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="P29">
+        <f t="shared" si="0"/>
+        <v>1348133400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3498,9 +3665,8 @@
       <c r="D30" t="s">
         <v>15</v>
       </c>
-      <c r="E30" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Sep-20 - 9:30 AM</v>
+      <c r="E30" s="1">
+        <v>41172.395833333336</v>
       </c>
       <c r="F30" t="s">
         <v>44</v>
@@ -3529,8 +3695,12 @@
       <c r="O30">
         <v>2363</v>
       </c>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="P30">
+        <f t="shared" si="0"/>
+        <v>1348219800</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3543,9 +3713,8 @@
       <c r="D31" t="s">
         <v>123</v>
       </c>
-      <c r="E31" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Sep-20 - 6:00 PM</v>
+      <c r="E31" s="1">
+        <v>41172.75</v>
       </c>
       <c r="F31" t="s">
         <v>124</v>
@@ -3568,8 +3737,12 @@
       <c r="O31">
         <v>2405</v>
       </c>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="P31">
+        <f t="shared" si="0"/>
+        <v>1348250400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3582,9 +3755,8 @@
       <c r="D32" t="s">
         <v>15</v>
       </c>
-      <c r="E32" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Sep-25 - 9:30 AM</v>
+      <c r="E32" s="1">
+        <v>41177.395833333336</v>
       </c>
       <c r="F32" t="s">
         <v>108</v>
@@ -3613,8 +3785,12 @@
       <c r="O32">
         <v>2349</v>
       </c>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="P32">
+        <f t="shared" si="0"/>
+        <v>1348651800</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3627,9 +3803,8 @@
       <c r="D33" t="s">
         <v>15</v>
       </c>
-      <c r="E33" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Sep-26 - 9:30 AM</v>
+      <c r="E33" s="1">
+        <v>41178.395833333336</v>
       </c>
       <c r="F33" t="s">
         <v>249</v>
@@ -3658,8 +3833,12 @@
       <c r="O33">
         <v>2404</v>
       </c>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="P33">
+        <f t="shared" si="0"/>
+        <v>1348738200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3672,9 +3851,8 @@
       <c r="D34" t="s">
         <v>15</v>
       </c>
-      <c r="E34" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Sep-27 - 9:30 AM</v>
+      <c r="E34" s="1">
+        <v>41179.395833333336</v>
       </c>
       <c r="F34" t="s">
         <v>257</v>
@@ -3703,8 +3881,12 @@
       <c r="O34">
         <v>2218</v>
       </c>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="P34">
+        <f t="shared" si="0"/>
+        <v>1348824600</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3717,9 +3899,8 @@
       <c r="D35" t="s">
         <v>15</v>
       </c>
-      <c r="E35" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Oct-02 - 9:30 AM</v>
+      <c r="E35" s="1">
+        <v>41184.395833333336</v>
       </c>
       <c r="F35" t="s">
         <v>265</v>
@@ -3748,8 +3929,12 @@
       <c r="O35">
         <v>2290</v>
       </c>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="P35">
+        <f t="shared" si="0"/>
+        <v>1349256600</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3762,9 +3947,8 @@
       <c r="D36" t="s">
         <v>15</v>
       </c>
-      <c r="E36" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Oct-03 - 9:30 AM</v>
+      <c r="E36" s="1">
+        <v>41185.395833333336</v>
       </c>
       <c r="F36" t="s">
         <v>92</v>
@@ -3793,8 +3977,12 @@
       <c r="O36">
         <v>2285</v>
       </c>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="P36">
+        <f t="shared" si="0"/>
+        <v>1349343000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3807,9 +3995,8 @@
       <c r="D37" t="s">
         <v>280</v>
       </c>
-      <c r="E37" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Oct-04 - 7:00 PM</v>
+      <c r="E37" s="1">
+        <v>41186.791666666664</v>
       </c>
       <c r="F37" t="s">
         <v>44</v>
@@ -3838,8 +4025,12 @@
       <c r="O37">
         <v>2206</v>
       </c>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="P37">
+        <f t="shared" si="0"/>
+        <v>1349463600</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3852,9 +4043,8 @@
       <c r="D38" t="s">
         <v>15</v>
       </c>
-      <c r="E38" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Oct-09 - 9:30 AM</v>
+      <c r="E38" s="1">
+        <v>41191.395833333336</v>
       </c>
       <c r="F38" t="s">
         <v>108</v>
@@ -3883,8 +4073,12 @@
       <c r="O38">
         <v>2284</v>
       </c>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="P38">
+        <f t="shared" si="0"/>
+        <v>1349861400</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3897,9 +4091,8 @@
       <c r="D39" t="s">
         <v>116</v>
       </c>
-      <c r="E39" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Oct-10 - 10:00 AM</v>
+      <c r="E39" s="1">
+        <v>41192.416666666664</v>
       </c>
       <c r="F39" t="s">
         <v>249</v>
@@ -3922,8 +4115,12 @@
       <c r="O39">
         <v>1897</v>
       </c>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="P39">
+        <f t="shared" si="0"/>
+        <v>1349949600</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3936,9 +4133,8 @@
       <c r="D40" t="s">
         <v>15</v>
       </c>
-      <c r="E40" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Oct-15 - 9:30 AM</v>
+      <c r="E40" s="1">
+        <v>41197.395833333336</v>
       </c>
       <c r="F40" t="s">
         <v>16</v>
@@ -3967,8 +4163,12 @@
       <c r="O40">
         <v>2149</v>
       </c>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="P40">
+        <f t="shared" si="0"/>
+        <v>1350379800</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3981,9 +4181,8 @@
       <c r="D41" t="s">
         <v>15</v>
       </c>
-      <c r="E41" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Oct-16 - 9:30 AM</v>
+      <c r="E41" s="1">
+        <v>41198.395833333336</v>
       </c>
       <c r="F41" t="s">
         <v>26</v>
@@ -4012,8 +4211,12 @@
       <c r="O41">
         <v>2229</v>
       </c>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="P41">
+        <f t="shared" si="0"/>
+        <v>1350466200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4026,9 +4229,8 @@
       <c r="D42" t="s">
         <v>15</v>
       </c>
-      <c r="E42" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Oct-17 - 9:30 AM</v>
+      <c r="E42" s="1">
+        <v>41199.395833333336</v>
       </c>
       <c r="F42" t="s">
         <v>26</v>
@@ -4057,8 +4259,12 @@
       <c r="O42">
         <v>2230</v>
       </c>
-    </row>
-    <row r="43" spans="1:15">
+      <c r="P42">
+        <f t="shared" si="0"/>
+        <v>1350552600</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4071,9 +4277,8 @@
       <c r="D43" t="s">
         <v>15</v>
       </c>
-      <c r="E43" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Oct-18 - 9:30 AM</v>
+      <c r="E43" s="1">
+        <v>41200.395833333336</v>
       </c>
       <c r="F43" t="s">
         <v>26</v>
@@ -4102,8 +4307,12 @@
       <c r="O43">
         <v>2237</v>
       </c>
-    </row>
-    <row r="44" spans="1:15">
+      <c r="P43">
+        <f t="shared" si="0"/>
+        <v>1350639000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4116,9 +4325,8 @@
       <c r="D44" t="s">
         <v>123</v>
       </c>
-      <c r="E44" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Oct-18 - 6:00 PM</v>
+      <c r="E44" s="1">
+        <v>41200.75</v>
       </c>
       <c r="F44" t="s">
         <v>124</v>
@@ -4141,8 +4349,12 @@
       <c r="O44">
         <v>2176</v>
       </c>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="P44">
+        <f t="shared" si="0"/>
+        <v>1350669600</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4155,9 +4367,8 @@
       <c r="D45" t="s">
         <v>15</v>
       </c>
-      <c r="E45" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Oct-23 - 9:30 AM</v>
+      <c r="E45" s="1">
+        <v>41205.395833333336</v>
       </c>
       <c r="F45" t="s">
         <v>26</v>
@@ -4186,8 +4397,12 @@
       <c r="O45">
         <v>2245</v>
       </c>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="P45">
+        <f t="shared" si="0"/>
+        <v>1351071000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4200,9 +4415,8 @@
       <c r="D46" t="s">
         <v>116</v>
       </c>
-      <c r="E46" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Oct-24 - 10:00 AM</v>
+      <c r="E46" s="1">
+        <v>41206.416666666664</v>
       </c>
       <c r="F46" t="s">
         <v>117</v>
@@ -4219,8 +4433,12 @@
       <c r="O46">
         <v>2495</v>
       </c>
-    </row>
-    <row r="47" spans="1:15">
+      <c r="P46">
+        <f t="shared" si="0"/>
+        <v>1351159200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4233,9 +4451,8 @@
       <c r="D47" t="s">
         <v>341</v>
       </c>
-      <c r="E47" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Oct-24 - 3:30 PM</v>
+      <c r="E47" s="1">
+        <v>41206.645833333336</v>
       </c>
       <c r="F47" t="s">
         <v>257</v>
@@ -4264,8 +4481,12 @@
       <c r="O47">
         <v>2236</v>
       </c>
-    </row>
-    <row r="48" spans="1:15">
+      <c r="P47">
+        <f t="shared" si="0"/>
+        <v>1351179000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4278,9 +4499,8 @@
       <c r="D48" t="s">
         <v>15</v>
       </c>
-      <c r="E48" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Nov-01 - 9:30 AM</v>
+      <c r="E48" s="1">
+        <v>41214.395833333336</v>
       </c>
       <c r="F48" t="s">
         <v>44</v>
@@ -4309,8 +4529,12 @@
       <c r="O48">
         <v>2267</v>
       </c>
-    </row>
-    <row r="49" spans="1:15">
+      <c r="P48">
+        <f t="shared" si="0"/>
+        <v>1351848600</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4323,9 +4547,8 @@
       <c r="D49" t="s">
         <v>15</v>
       </c>
-      <c r="E49" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Nov-01 - 9:30 AM</v>
+      <c r="E49" s="1">
+        <v>41214.395833333336</v>
       </c>
       <c r="F49" t="s">
         <v>124</v>
@@ -4342,8 +4565,12 @@
       <c r="O49">
         <v>2397</v>
       </c>
-    </row>
-    <row r="50" spans="1:15">
+      <c r="P49">
+        <f t="shared" si="0"/>
+        <v>1351848600</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4356,9 +4583,8 @@
       <c r="D50" t="s">
         <v>15</v>
       </c>
-      <c r="E50" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Nov-06 - 9:30 AM</v>
+      <c r="E50" s="1">
+        <v>41219.395833333336</v>
       </c>
       <c r="F50" t="s">
         <v>83</v>
@@ -4387,8 +4613,12 @@
       <c r="O50">
         <v>2150</v>
       </c>
-    </row>
-    <row r="51" spans="1:15">
+      <c r="P50">
+        <f t="shared" si="0"/>
+        <v>1352280600</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4401,9 +4631,8 @@
       <c r="D51" t="s">
         <v>15</v>
       </c>
-      <c r="E51" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Nov-07 - 9:30 AM</v>
+      <c r="E51" s="1">
+        <v>41220.395833333336</v>
       </c>
       <c r="F51" t="s">
         <v>16</v>
@@ -4432,8 +4661,12 @@
       <c r="O51">
         <v>2178</v>
       </c>
-    </row>
-    <row r="52" spans="1:15">
+      <c r="P51">
+        <f t="shared" si="0"/>
+        <v>1352367000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4446,9 +4679,8 @@
       <c r="D52" t="s">
         <v>15</v>
       </c>
-      <c r="E52" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Nov-13 - 9:30 AM</v>
+      <c r="E52" s="1">
+        <v>41226.395833333336</v>
       </c>
       <c r="F52" t="s">
         <v>130</v>
@@ -4477,8 +4709,12 @@
       <c r="O52">
         <v>2266</v>
       </c>
-    </row>
-    <row r="53" spans="1:15">
+      <c r="P52">
+        <f t="shared" si="0"/>
+        <v>1352885400</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4491,9 +4727,8 @@
       <c r="D53" t="s">
         <v>116</v>
       </c>
-      <c r="E53" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Nov-14 - 10:00 AM</v>
+      <c r="E53" s="1">
+        <v>41227.416666666664</v>
       </c>
       <c r="F53" t="s">
         <v>249</v>
@@ -4516,8 +4751,12 @@
       <c r="O53">
         <v>2139</v>
       </c>
-    </row>
-    <row r="54" spans="1:15">
+      <c r="P53">
+        <f t="shared" si="0"/>
+        <v>1352973600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4530,9 +4769,8 @@
       <c r="D54" t="s">
         <v>15</v>
       </c>
-      <c r="E54" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Nov-15 - 9:30 AM</v>
+      <c r="E54" s="1">
+        <v>41228.395833333336</v>
       </c>
       <c r="F54" t="s">
         <v>44</v>
@@ -4561,8 +4799,12 @@
       <c r="O54">
         <v>2268</v>
       </c>
-    </row>
-    <row r="55" spans="1:15">
+      <c r="P54">
+        <f t="shared" si="0"/>
+        <v>1353058200</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4575,9 +4817,8 @@
       <c r="D55" t="s">
         <v>15</v>
       </c>
-      <c r="E55" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Nov-16 - 9:30 AM</v>
+      <c r="E55" s="1">
+        <v>41229.395833333336</v>
       </c>
       <c r="F55" t="s">
         <v>392</v>
@@ -4600,8 +4841,12 @@
       <c r="O55">
         <v>2227</v>
       </c>
-    </row>
-    <row r="56" spans="1:15">
+      <c r="P55">
+        <f t="shared" si="0"/>
+        <v>1353144600</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4614,9 +4859,8 @@
       <c r="D56" t="s">
         <v>15</v>
       </c>
-      <c r="E56" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Nov-19 - 9:30 AM</v>
+      <c r="E56" s="1">
+        <v>41232.395833333336</v>
       </c>
       <c r="F56" t="s">
         <v>398</v>
@@ -4645,8 +4889,12 @@
       <c r="O56">
         <v>2274</v>
       </c>
-    </row>
-    <row r="57" spans="1:15">
+      <c r="P56">
+        <f t="shared" si="0"/>
+        <v>1353403800</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4659,9 +4907,8 @@
       <c r="D57" t="s">
         <v>15</v>
       </c>
-      <c r="E57" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Nov-20 - 9:30 AM</v>
+      <c r="E57" s="1">
+        <v>41233.395833333336</v>
       </c>
       <c r="F57" t="s">
         <v>153</v>
@@ -4690,8 +4937,12 @@
       <c r="O57">
         <v>2269</v>
       </c>
-    </row>
-    <row r="58" spans="1:15">
+      <c r="P57">
+        <f t="shared" si="0"/>
+        <v>1353490200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4704,9 +4955,8 @@
       <c r="D58" t="s">
         <v>15</v>
       </c>
-      <c r="E58" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Nov-21 - 9:30 AM</v>
+      <c r="E58" s="1">
+        <v>41234.395833333336</v>
       </c>
       <c r="F58" t="s">
         <v>35</v>
@@ -4735,8 +4985,12 @@
       <c r="O58">
         <v>2273</v>
       </c>
-    </row>
-    <row r="59" spans="1:15">
+      <c r="P58">
+        <f t="shared" si="0"/>
+        <v>1353576600</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4749,9 +5003,8 @@
       <c r="D59" t="s">
         <v>15</v>
       </c>
-      <c r="E59" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Nov-27 - 9:30 AM</v>
+      <c r="E59" s="1">
+        <v>41240.395833333336</v>
       </c>
       <c r="F59" t="s">
         <v>420</v>
@@ -4780,8 +5033,12 @@
       <c r="O59">
         <v>2281</v>
       </c>
-    </row>
-    <row r="60" spans="1:15">
+      <c r="P59">
+        <f t="shared" si="0"/>
+        <v>1354095000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4794,9 +5051,8 @@
       <c r="D60" t="s">
         <v>116</v>
       </c>
-      <c r="E60" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Nov-28 - 10:00 AM</v>
+      <c r="E60" s="1">
+        <v>41241.416666666664</v>
       </c>
       <c r="F60" t="s">
         <v>249</v>
@@ -4819,8 +5075,12 @@
       <c r="O60">
         <v>2413</v>
       </c>
-    </row>
-    <row r="61" spans="1:15">
+      <c r="P60">
+        <f t="shared" si="0"/>
+        <v>1354183200</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4833,9 +5093,8 @@
       <c r="D61" t="s">
         <v>433</v>
       </c>
-      <c r="E61" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Nov-29 - 1:30 PM</v>
+      <c r="E61" s="1">
+        <v>41242.5625</v>
       </c>
       <c r="F61" t="s">
         <v>100</v>
@@ -4858,8 +5117,12 @@
       <c r="O61">
         <v>2226</v>
       </c>
-    </row>
-    <row r="62" spans="1:15">
+      <c r="P61">
+        <f t="shared" si="0"/>
+        <v>1354282200</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4872,9 +5135,8 @@
       <c r="D62" t="s">
         <v>15</v>
       </c>
-      <c r="E62" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Dec-04 - 9:30 AM</v>
+      <c r="E62" s="1">
+        <v>41247.395833333336</v>
       </c>
       <c r="F62" t="s">
         <v>83</v>
@@ -4903,8 +5165,12 @@
       <c r="O62">
         <v>2270</v>
       </c>
-    </row>
-    <row r="63" spans="1:15">
+      <c r="P62">
+        <f t="shared" si="0"/>
+        <v>1354699800</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4917,9 +5183,8 @@
       <c r="D63" t="s">
         <v>446</v>
       </c>
-      <c r="E63" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Dec-05 - 12:00 PM</v>
+      <c r="E63" s="1">
+        <v>41248.5</v>
       </c>
       <c r="F63" t="s">
         <v>447</v>
@@ -4948,8 +5213,12 @@
       <c r="O63">
         <v>2283</v>
       </c>
-    </row>
-    <row r="64" spans="1:15">
+      <c r="P63">
+        <f t="shared" si="0"/>
+        <v>1354795200</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4962,9 +5231,8 @@
       <c r="D64" t="s">
         <v>15</v>
       </c>
-      <c r="E64" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Dec-06 - 9:30 AM</v>
+      <c r="E64" s="1">
+        <v>41249.395833333336</v>
       </c>
       <c r="F64" t="s">
         <v>455</v>
@@ -4993,8 +5261,12 @@
       <c r="O64">
         <v>2279</v>
       </c>
-    </row>
-    <row r="65" spans="1:15">
+      <c r="P64">
+        <f t="shared" si="0"/>
+        <v>1354872600</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
       <c r="A65">
         <v>64</v>
       </c>
@@ -5007,9 +5279,8 @@
       <c r="D65" t="s">
         <v>463</v>
       </c>
-      <c r="E65" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Dec-10 - 1:00 PM</v>
+      <c r="E65" s="1">
+        <v>41253.541666666664</v>
       </c>
       <c r="F65" t="s">
         <v>16</v>
@@ -5038,8 +5309,12 @@
       <c r="O65">
         <v>2442</v>
       </c>
-    </row>
-    <row r="66" spans="1:15">
+      <c r="P65">
+        <f t="shared" si="0"/>
+        <v>1355230800</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5052,9 +5327,8 @@
       <c r="D66" t="s">
         <v>15</v>
       </c>
-      <c r="E66" t="str">
-        <f t="shared" si="0"/>
-        <v>2012-Dec-11 - 9:30 AM</v>
+      <c r="E66" s="1">
+        <v>41254.395833333336</v>
       </c>
       <c r="F66" t="s">
         <v>130</v>
@@ -5083,8 +5357,12 @@
       <c r="O66">
         <v>2282</v>
       </c>
-    </row>
-    <row r="67" spans="1:15">
+      <c r="P66">
+        <f t="shared" si="0"/>
+        <v>1355304600</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
       <c r="A67">
         <v>66</v>
       </c>
@@ -5097,9 +5375,8 @@
       <c r="D67" t="s">
         <v>116</v>
       </c>
-      <c r="E67" t="str">
-        <f t="shared" ref="E67:E87" si="1">C67&amp;" - "&amp;D67</f>
-        <v>2012-Dec-12 - 10:00 AM</v>
+      <c r="E67" s="1">
+        <v>41255.416666666664</v>
       </c>
       <c r="F67" t="s">
         <v>478</v>
@@ -5122,8 +5399,12 @@
       <c r="O67">
         <v>2447</v>
       </c>
-    </row>
-    <row r="68" spans="1:15">
+      <c r="P67">
+        <f t="shared" ref="P67:P87" si="1" xml:space="preserve"> (E67 * 86400) - 2209075200</f>
+        <v>1355392800</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5136,9 +5417,8 @@
       <c r="D68" t="s">
         <v>116</v>
       </c>
-      <c r="E68" t="str">
-        <f t="shared" si="1"/>
-        <v>2012-Dec-13 - 10:00 AM</v>
+      <c r="E68" s="1">
+        <v>41256.416666666664</v>
       </c>
       <c r="F68" t="s">
         <v>249</v>
@@ -5155,8 +5435,12 @@
       <c r="O68">
         <v>2446</v>
       </c>
-    </row>
-    <row r="69" spans="1:15">
+      <c r="P68">
+        <f t="shared" si="1"/>
+        <v>1355479200</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16">
       <c r="A69">
         <v>68</v>
       </c>
@@ -5169,9 +5453,8 @@
       <c r="D69" t="s">
         <v>116</v>
       </c>
-      <c r="E69" t="str">
-        <f t="shared" si="1"/>
-        <v>2012-Dec-19 - 10:00 AM</v>
+      <c r="E69" s="1">
+        <v>41262.416666666664</v>
       </c>
       <c r="F69" t="s">
         <v>249</v>
@@ -5194,8 +5477,12 @@
       <c r="O69">
         <v>2439</v>
       </c>
-    </row>
-    <row r="70" spans="1:15">
+      <c r="P69">
+        <f t="shared" si="1"/>
+        <v>1355997600</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
       <c r="A70">
         <v>69</v>
       </c>
@@ -5208,9 +5495,8 @@
       <c r="D70" t="s">
         <v>116</v>
       </c>
-      <c r="E70" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Jan-09 - 10:00 AM</v>
+      <c r="E70" s="1">
+        <v>41283.416666666664</v>
       </c>
       <c r="F70" t="s">
         <v>494</v>
@@ -5227,8 +5513,12 @@
       <c r="O70">
         <v>2483</v>
       </c>
-    </row>
-    <row r="71" spans="1:15">
+      <c r="P70">
+        <f t="shared" si="1"/>
+        <v>1357812000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16">
       <c r="A71">
         <v>70</v>
       </c>
@@ -5241,9 +5531,8 @@
       <c r="D71" t="s">
         <v>15</v>
       </c>
-      <c r="E71" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Jan-14 - 9:30 AM</v>
+      <c r="E71" s="1">
+        <v>41288.395833333336</v>
       </c>
       <c r="F71" t="s">
         <v>498</v>
@@ -5272,8 +5561,12 @@
       <c r="O71">
         <v>2406</v>
       </c>
-    </row>
-    <row r="72" spans="1:15">
+      <c r="P71">
+        <f t="shared" si="1"/>
+        <v>1358242200</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16">
       <c r="A72">
         <v>71</v>
       </c>
@@ -5286,9 +5579,8 @@
       <c r="D72" t="s">
         <v>15</v>
       </c>
-      <c r="E72" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Jan-15 - 9:30 AM</v>
+      <c r="E72" s="1">
+        <v>41289.395833333336</v>
       </c>
       <c r="F72" t="s">
         <v>506</v>
@@ -5317,8 +5609,12 @@
       <c r="O72">
         <v>2292</v>
       </c>
-    </row>
-    <row r="73" spans="1:15">
+      <c r="P72">
+        <f t="shared" si="1"/>
+        <v>1358328600</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16">
       <c r="A73">
         <v>72</v>
       </c>
@@ -5331,9 +5627,8 @@
       <c r="D73" t="s">
         <v>15</v>
       </c>
-      <c r="E73" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Jan-16 - 9:30 AM</v>
+      <c r="E73" s="1">
+        <v>41290.395833333336</v>
       </c>
       <c r="F73" t="s">
         <v>514</v>
@@ -5362,8 +5657,12 @@
       <c r="O73">
         <v>2271</v>
       </c>
-    </row>
-    <row r="74" spans="1:15">
+      <c r="P73">
+        <f t="shared" si="1"/>
+        <v>1358415000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16">
       <c r="A74">
         <v>73</v>
       </c>
@@ -5376,9 +5675,8 @@
       <c r="D74" t="s">
         <v>15</v>
       </c>
-      <c r="E74" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Jan-17 - 9:30 AM</v>
+      <c r="E74" s="1">
+        <v>41291.395833333336</v>
       </c>
       <c r="F74" t="s">
         <v>392</v>
@@ -5407,8 +5705,12 @@
       <c r="O74">
         <v>2438</v>
       </c>
-    </row>
-    <row r="75" spans="1:15">
+      <c r="P74">
+        <f t="shared" si="1"/>
+        <v>1358501400</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16">
       <c r="A75">
         <v>74</v>
       </c>
@@ -5421,9 +5723,8 @@
       <c r="D75" t="s">
         <v>433</v>
       </c>
-      <c r="E75" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Jan-17 - 1:30 PM</v>
+      <c r="E75" s="1">
+        <v>41291.5625</v>
       </c>
       <c r="F75" t="s">
         <v>44</v>
@@ -5446,8 +5747,12 @@
       <c r="O75">
         <v>2431</v>
       </c>
-    </row>
-    <row r="76" spans="1:15">
+      <c r="P75">
+        <f t="shared" si="1"/>
+        <v>1358515800</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16">
       <c r="A76">
         <v>75</v>
       </c>
@@ -5460,9 +5765,8 @@
       <c r="D76" t="s">
         <v>123</v>
       </c>
-      <c r="E76" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Jan-17 - 6:00 PM</v>
+      <c r="E76" s="1">
+        <v>41291.75</v>
       </c>
       <c r="F76" t="s">
         <v>532</v>
@@ -5479,8 +5783,12 @@
       <c r="O76">
         <v>2452</v>
       </c>
-    </row>
-    <row r="77" spans="1:15">
+      <c r="P76">
+        <f t="shared" si="1"/>
+        <v>1358532000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16">
       <c r="A77">
         <v>76</v>
       </c>
@@ -5493,9 +5801,8 @@
       <c r="D77" t="s">
         <v>15</v>
       </c>
-      <c r="E77" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Jan-21 - 9:30 AM</v>
+      <c r="E77" s="1">
+        <v>41295.395833333336</v>
       </c>
       <c r="F77" t="s">
         <v>83</v>
@@ -5524,8 +5831,12 @@
       <c r="O77">
         <v>2424</v>
       </c>
-    </row>
-    <row r="78" spans="1:15">
+      <c r="P77">
+        <f t="shared" si="1"/>
+        <v>1358847000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16">
       <c r="A78">
         <v>77</v>
       </c>
@@ -5538,9 +5849,8 @@
       <c r="D78" t="s">
         <v>116</v>
       </c>
-      <c r="E78" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Jan-23 - 10:00 AM</v>
+      <c r="E78" s="1">
+        <v>41297.416666666664</v>
       </c>
       <c r="F78" t="s">
         <v>249</v>
@@ -5566,8 +5876,12 @@
       <c r="O78">
         <v>2480</v>
       </c>
-    </row>
-    <row r="79" spans="1:15">
+      <c r="P78">
+        <f t="shared" si="1"/>
+        <v>1359021600</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5580,9 +5894,8 @@
       <c r="D79" t="s">
         <v>116</v>
       </c>
-      <c r="E79" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Jan-30 - 10:00 AM</v>
+      <c r="E79" s="1">
+        <v>41304.416666666664</v>
       </c>
       <c r="F79" t="s">
         <v>550</v>
@@ -5599,8 +5912,12 @@
       <c r="O79">
         <v>2486</v>
       </c>
-    </row>
-    <row r="80" spans="1:15">
+      <c r="P79">
+        <f t="shared" si="1"/>
+        <v>1359626400</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5613,9 +5930,8 @@
       <c r="D80" t="s">
         <v>15</v>
       </c>
-      <c r="E80" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Feb-05 - 9:30 AM</v>
+      <c r="E80" s="1">
+        <v>41310.395833333336</v>
       </c>
       <c r="F80" t="s">
         <v>83</v>
@@ -5641,8 +5957,12 @@
       <c r="O80">
         <v>2347</v>
       </c>
-    </row>
-    <row r="81" spans="1:15">
+      <c r="P80">
+        <f t="shared" si="1"/>
+        <v>1360143000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16">
       <c r="A81">
         <v>80</v>
       </c>
@@ -5655,9 +5975,8 @@
       <c r="D81" t="s">
         <v>15</v>
       </c>
-      <c r="E81" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Feb-06 - 9:30 AM</v>
+      <c r="E81" s="1">
+        <v>41311.395833333336</v>
       </c>
       <c r="F81" t="s">
         <v>559</v>
@@ -5683,8 +6002,12 @@
       <c r="O81">
         <v>2233</v>
       </c>
-    </row>
-    <row r="82" spans="1:15">
+      <c r="P81">
+        <f t="shared" si="1"/>
+        <v>1360229400</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5697,9 +6020,8 @@
       <c r="D82" t="s">
         <v>15</v>
       </c>
-      <c r="E82" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Feb-07 - 9:30 AM</v>
+      <c r="E82" s="1">
+        <v>41312.395833333336</v>
       </c>
       <c r="F82" t="s">
         <v>565</v>
@@ -5725,8 +6047,12 @@
       <c r="O82">
         <v>2316</v>
       </c>
-    </row>
-    <row r="83" spans="1:15">
+      <c r="P82">
+        <f t="shared" si="1"/>
+        <v>1360315800</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5739,9 +6065,8 @@
       <c r="D83" t="s">
         <v>15</v>
       </c>
-      <c r="E83" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Feb-12 - 9:30 AM</v>
+      <c r="E83" s="1">
+        <v>41317.395833333336</v>
       </c>
       <c r="F83" t="s">
         <v>571</v>
@@ -5767,8 +6092,12 @@
       <c r="O83">
         <v>2326</v>
       </c>
-    </row>
-    <row r="84" spans="1:15">
+      <c r="P83">
+        <f t="shared" si="1"/>
+        <v>1360747800</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5781,9 +6110,8 @@
       <c r="D84" t="s">
         <v>116</v>
       </c>
-      <c r="E84" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Feb-13 - 10:00 AM</v>
+      <c r="E84" s="1">
+        <v>41318.416666666664</v>
       </c>
       <c r="F84" t="s">
         <v>249</v>
@@ -5809,8 +6137,12 @@
       <c r="O84">
         <v>2479</v>
       </c>
-    </row>
-    <row r="85" spans="1:15">
+      <c r="P84">
+        <f t="shared" si="1"/>
+        <v>1360836000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5823,9 +6155,8 @@
       <c r="D85" t="s">
         <v>15</v>
       </c>
-      <c r="E85" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Feb-19 - 9:30 AM</v>
+      <c r="E85" s="1">
+        <v>41324.395833333336</v>
       </c>
       <c r="F85" t="s">
         <v>582</v>
@@ -5851,8 +6182,12 @@
       <c r="O85">
         <v>2398</v>
       </c>
-    </row>
-    <row r="86" spans="1:15">
+      <c r="P85">
+        <f t="shared" si="1"/>
+        <v>1361352600</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5865,9 +6200,8 @@
       <c r="D86" t="s">
         <v>15</v>
       </c>
-      <c r="E86" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Feb-20 - 9:30 AM</v>
+      <c r="E86" s="1">
+        <v>41325.395833333336</v>
       </c>
       <c r="F86" t="s">
         <v>514</v>
@@ -5893,8 +6227,12 @@
       <c r="O86">
         <v>2272</v>
       </c>
-    </row>
-    <row r="87" spans="1:15">
+      <c r="P86">
+        <f t="shared" si="1"/>
+        <v>1361439000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5907,9 +6245,8 @@
       <c r="D87" t="s">
         <v>15</v>
       </c>
-      <c r="E87" t="str">
-        <f t="shared" si="1"/>
-        <v>2013-Feb-21 - 9:30 AM</v>
+      <c r="E87" s="1">
+        <v>41326.395833333336</v>
       </c>
       <c r="F87" t="s">
         <v>44</v>
@@ -5931,6 +6268,10 @@
       </c>
       <c r="O87">
         <v>2333</v>
+      </c>
+      <c r="P87">
+        <f t="shared" si="1"/>
+        <v>1361525400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>